<commit_message>
Added ticket OmegaT #1171
</commit_message>
<xml_diff>
--- a/tickets/OmegaT_issues_nopw.xlsx
+++ b/tickets/OmegaT_issues_nopw.xlsx
@@ -13,7 +13,7 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$99</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$100</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"Devs"</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="236">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -138,6 +138,15 @@
     <t xml:space="preserve">The COMPILE event is fired *after* the target commit</t>
   </si>
   <si>
+    <t xml:space="preserve">#1171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enforced translations lose background color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
     <t xml:space="preserve">#1164</t>
   </si>
   <si>
@@ -157,9 +166,6 @@
   </si>
   <si>
     <t xml:space="preserve">RFE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
   </si>
   <si>
     <t xml:space="preserve">#1163</t>
@@ -1363,7 +1369,7 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ101"/>
+  <dimension ref="A1:AMJ102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1472,7 +1478,7 @@
     </row>
     <row r="6" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
-        <v>45049</v>
+        <v>45064</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>35</v>
@@ -1500,17 +1506,17 @@
       <c r="B7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="E7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
@@ -1518,22 +1524,22 @@
     </row>
     <row r="8" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
-        <v>45044</v>
+        <v>45049</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="F8" s="9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
@@ -1541,7 +1547,7 @@
     </row>
     <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
-        <v>45040</v>
+        <v>45044</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>45</v>
@@ -1556,7 +1562,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
@@ -1564,7 +1570,7 @@
     </row>
     <row r="10" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>47</v>
@@ -1576,10 +1582,10 @@
         <v>48</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
@@ -1587,16 +1593,22 @@
     </row>
     <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="C11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="E11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>49</v>
       </c>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
@@ -1604,22 +1616,16 @@
     </row>
     <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B12" s="11" t="s">
+        <v>44996</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="F12" s="9" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
@@ -1627,7 +1633,7 @@
     </row>
     <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>54</v>
@@ -1642,7 +1648,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
@@ -1673,13 +1679,13 @@
     </row>
     <row r="15" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>59</v>
@@ -1688,7 +1694,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
@@ -1696,22 +1702,22 @@
     </row>
     <row r="16" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
@@ -1719,7 +1725,7 @@
     </row>
     <row r="17" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
-        <v>44972</v>
+        <v>44981</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>63</v>
@@ -1731,33 +1737,33 @@
         <v>64</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
       <c r="AMJ17" s="0"/>
     </row>
-    <row r="18" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B18" s="14" t="s">
+    <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>42</v>
+      <c r="E18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
@@ -1765,22 +1771,22 @@
     </row>
     <row r="19" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>67</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>68</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
@@ -1788,22 +1794,22 @@
     </row>
     <row r="20" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="E20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
@@ -1811,7 +1817,7 @@
     </row>
     <row r="21" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>72</v>
@@ -1823,7 +1829,7 @@
         <v>73</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>32</v>
@@ -1846,10 +1852,10 @@
         <v>75</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
@@ -1857,22 +1863,22 @@
     </row>
     <row r="23" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="n">
-        <v>44949</v>
+        <v>44952</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>78</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>69</v>
       </c>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
@@ -1880,22 +1886,22 @@
     </row>
     <row r="24" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="n">
-        <v>44948</v>
+        <v>44949</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>79</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>80</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
@@ -1903,125 +1909,125 @@
     </row>
     <row r="25" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>82</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AMH25" s="0"/>
       <c r="AMI25" s="0"/>
       <c r="AMJ25" s="0"/>
     </row>
-    <row r="26" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B26" s="16" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="E26" s="12" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
-    <row r="27" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+    <row r="27" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B27" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>29</v>
+      <c r="C27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="5" t="s">
+    <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>42</v>
+      <c r="F28" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B29" s="14" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="C29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>42</v>
+      <c r="E29" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B30" s="17" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B30" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>32</v>
+      <c r="E30" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
@@ -2029,7 +2035,7 @@
     </row>
     <row r="31" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>93</v>
@@ -2041,112 +2047,115 @@
         <v>94</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
-    <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B32" s="18" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="E32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>76</v>
-      </c>
+      <c r="AMH32" s="0"/>
+      <c r="AMI32" s="0"/>
+      <c r="AMJ32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B33" s="17" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>100</v>
       </c>
       <c r="E33" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13" t="n">
+        <v>373466</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="n">
-        <v>44743</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="F34" s="5" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>102</v>
+        <v>44743</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="F35" s="5" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B36" s="20" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>104</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>105</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>106</v>
@@ -2158,90 +2167,90 @@
         <v>107</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B38" s="21" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B38" s="20" t="s">
         <v>108</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>109</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="n">
-        <v>44659</v>
+        <v>44695</v>
       </c>
       <c r="B39" s="21" t="s">
         <v>110</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>111</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B40" s="20" t="s">
+        <v>44659</v>
+      </c>
+      <c r="B40" s="21" t="s">
         <v>112</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B41" s="17" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="E41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2258,15 +2267,15 @@
         <v>118</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="13" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>119</v>
@@ -2278,15 +2287,15 @@
         <v>120</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>121</v>
@@ -2298,57 +2307,57 @@
         <v>122</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="13" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>123</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>124</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>125</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>126</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B47" s="20" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B47" s="17" t="s">
         <v>127</v>
       </c>
       <c r="C47" s="5" t="s">
@@ -2358,60 +2367,60 @@
         <v>128</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B48" s="17" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>129</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>130</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="13" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="13" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B50" s="17" t="s">
+      <c r="C49" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="5" t="s">
+      <c r="E49" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="13" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>134</v>
@@ -2423,10 +2432,10 @@
         <v>135</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>136</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2434,24 +2443,24 @@
         <v>44460</v>
       </c>
       <c r="B52" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="E52" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="13" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B53" s="17" t="s">
         <v>139</v>
@@ -2466,72 +2475,72 @@
         <v>23</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="13" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>141</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>142</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="13" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B55" s="21" t="s">
+        <v>44326</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>143</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>144</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="13" t="n">
         <v>44325</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="21" t="s">
         <v>145</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>146</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="13" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>147</v>
@@ -2543,15 +2552,15 @@
         <v>148</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="13" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>149</v>
@@ -2563,37 +2572,37 @@
         <v>150</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>151</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="13" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B59" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D59" s="5" t="s">
+      <c r="E59" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F59" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B60" s="17" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>154</v>
       </c>
       <c r="C60" s="5" t="s">
@@ -2603,15 +2612,15 @@
         <v>155</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="13" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>156</v>
@@ -2623,57 +2632,57 @@
         <v>157</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="22" t="n">
+      <c r="A62" s="13" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="22" t="n">
         <v>44231</v>
       </c>
-      <c r="B62" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="E62" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F62" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="13" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="5" t="s">
+      <c r="C63" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F63" s="24" t="s">
         <v>161</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="13" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B64" s="20" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B64" s="17" t="s">
         <v>162</v>
       </c>
       <c r="C64" s="5" t="s">
@@ -2683,17 +2692,17 @@
         <v>163</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="13" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B65" s="17" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B65" s="20" t="s">
         <v>164</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2703,10 +2712,10 @@
         <v>165</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,40 +2732,40 @@
         <v>167</v>
       </c>
       <c r="E66" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="13" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F66" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="13" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>42</v>
+      <c r="F67" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="13" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>170</v>
@@ -2765,158 +2774,158 @@
         <v>7</v>
       </c>
       <c r="D69" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="13" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E69" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="22" t="n">
+      <c r="E70" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="22" t="n">
         <v>44146</v>
       </c>
-      <c r="B70" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="C70" s="24" t="s">
+      <c r="B71" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="C71" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D70" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="E70" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="13" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="E71" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>42</v>
+      <c r="E71" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F71" s="24" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="13" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>176</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="22" t="n">
+      <c r="A73" s="13" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="22" t="n">
         <v>44095</v>
       </c>
-      <c r="B73" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="C73" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="E73" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="13" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="23" t="s">
         <v>179</v>
       </c>
-      <c r="C74" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="5" t="s">
+      <c r="C74" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="E74" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>42</v>
+      <c r="E74" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="13" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B75" s="17" t="s">
         <v>181</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>182</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>136</v>
+        <v>37</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="13" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B76" s="17" t="s">
         <v>183</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>184</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="13" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B77" s="17" t="s">
         <v>185</v>
@@ -2928,15 +2937,15 @@
         <v>186</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="13" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>187</v>
@@ -2948,15 +2957,15 @@
         <v>188</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="13" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>189</v>
@@ -2968,15 +2977,15 @@
         <v>190</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B80" s="17" t="s">
         <v>191</v>
@@ -2988,35 +2997,35 @@
         <v>192</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="13" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>193</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>194</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="13" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B82" s="17" t="s">
         <v>195</v>
@@ -3028,15 +3037,15 @@
         <v>196</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="13" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B83" s="17" t="s">
         <v>197</v>
@@ -3048,15 +3057,15 @@
         <v>198</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="13" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B84" s="17" t="s">
         <v>199</v>
@@ -3068,35 +3077,35 @@
         <v>200</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="13" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B85" s="17" t="s">
         <v>201</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>202</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="13" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>203</v>
@@ -3108,15 +3117,15 @@
         <v>204</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="13" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B87" s="17" t="s">
         <v>205</v>
@@ -3128,15 +3137,15 @@
         <v>206</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="13" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B88" s="17" t="s">
         <v>207</v>
@@ -3148,10 +3157,10 @@
         <v>208</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,15 +3177,15 @@
         <v>210</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="13" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B90" s="17" t="s">
         <v>211</v>
@@ -3188,15 +3197,15 @@
         <v>212</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="13" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B91" s="17" t="s">
         <v>213</v>
@@ -3208,10 +3217,10 @@
         <v>214</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3231,14 +3240,14 @@
         <v>23</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="13" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B93" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B93" s="17" t="s">
         <v>217</v>
       </c>
       <c r="C93" s="5" t="s">
@@ -3251,32 +3260,32 @@
         <v>23</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="13" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B95" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="13" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="C95" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D95" s="5" t="s">
+      <c r="C94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="E95" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>69</v>
+      <c r="E94" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3287,61 +3296,61 @@
         <v>221</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>222</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>223</v>
+        <v>71</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="13" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B97" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C97" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D97" s="5" t="s">
+      <c r="E97" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F97" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="13" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B98" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B98" s="25" t="s">
         <v>226</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>227</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="13" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>228</v>
@@ -3353,19 +3362,39 @@
         <v>229</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="101" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMH101" s="0"/>
-      <c r="AMI101" s="0"/>
-      <c r="AMJ101" s="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="13" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="102" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMH102" s="0"/>
+      <c r="AMI102" s="0"/>
+      <c r="AMJ102" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F99">
+  <autoFilter ref="A1:F100">
     <filterColumn colId="5">
       <filters>
         <filter val="Fixed?"/>
@@ -3388,94 +3417,95 @@
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="#1309"/>
     <hyperlink ref="B5" r:id="rId2" display="#1176"/>
-    <hyperlink ref="B6" r:id="rId3" display="#1164"/>
-    <hyperlink ref="B7" r:id="rId4" display="#9"/>
-    <hyperlink ref="B8" r:id="rId5" display="#1163"/>
-    <hyperlink ref="B9" r:id="rId6" display="#1161"/>
-    <hyperlink ref="B10" r:id="rId7" display="#1690"/>
-    <hyperlink ref="B12" r:id="rId8" display="#1155"/>
-    <hyperlink ref="B13" r:id="rId9" display="#1150"/>
-    <hyperlink ref="B14" r:id="rId10" display="#1151"/>
-    <hyperlink ref="B15" r:id="rId11" display="#1200"/>
-    <hyperlink ref="B16" r:id="rId12" display="#1681"/>
-    <hyperlink ref="B17" r:id="rId13" display="#1142"/>
-    <hyperlink ref="B18" r:id="rId14" display="#8"/>
-    <hyperlink ref="B19" r:id="rId15" display="#1674"/>
-    <hyperlink ref="B20" r:id="rId16" display="#1672"/>
-    <hyperlink ref="B21" r:id="rId17" display="#1669"/>
-    <hyperlink ref="B22" r:id="rId18" display="#1670"/>
-    <hyperlink ref="B23" r:id="rId19" display="#1184"/>
-    <hyperlink ref="B24" r:id="rId20" display="#49"/>
-    <hyperlink ref="B25" r:id="rId21" display="#1140"/>
-    <hyperlink ref="B26" r:id="rId22" display="#1132"/>
-    <hyperlink ref="B28" r:id="rId23" display="#1125"/>
-    <hyperlink ref="B29" r:id="rId24" display="#1641"/>
-    <hyperlink ref="B30" r:id="rId25" display="#1124"/>
-    <hyperlink ref="B31" r:id="rId26" display="#1122"/>
-    <hyperlink ref="B32" r:id="rId27" display="#43"/>
-    <hyperlink ref="B33" r:id="rId28" display="#1622"/>
-    <hyperlink ref="B35" r:id="rId29" display="#38"/>
-    <hyperlink ref="B36" r:id="rId30" display="#1621"/>
-    <hyperlink ref="B37" r:id="rId31" display="#1616"/>
-    <hyperlink ref="B38" r:id="rId32" display="#37"/>
-    <hyperlink ref="B39" r:id="rId33" display="#36"/>
-    <hyperlink ref="B40" r:id="rId34" display="#1101"/>
-    <hyperlink ref="B41" r:id="rId35" display="#1099"/>
-    <hyperlink ref="B42" r:id="rId36" display="#1098"/>
-    <hyperlink ref="B43" r:id="rId37" display="#1617"/>
-    <hyperlink ref="B44" r:id="rId38" display="#1092"/>
-    <hyperlink ref="B45" r:id="rId39" display="#1128"/>
-    <hyperlink ref="B46" r:id="rId40" display="#1090"/>
-    <hyperlink ref="B47" r:id="rId41" display="#1608"/>
-    <hyperlink ref="B48" r:id="rId42" display="#35"/>
-    <hyperlink ref="B50" r:id="rId43" display="#1070"/>
-    <hyperlink ref="B51" r:id="rId44" display="#1592"/>
-    <hyperlink ref="B52" r:id="rId45" display="#1591"/>
-    <hyperlink ref="B53" r:id="rId46" display="#1578"/>
-    <hyperlink ref="B54" r:id="rId47" display="#41"/>
-    <hyperlink ref="B55" r:id="rId48" display="#42"/>
-    <hyperlink ref="B56" r:id="rId49" display="#1566"/>
-    <hyperlink ref="B57" r:id="rId50" display="#1565"/>
-    <hyperlink ref="B58" r:id="rId51" display="#1046"/>
-    <hyperlink ref="B59" r:id="rId52" display="#1559"/>
-    <hyperlink ref="B60" r:id="rId53" display="#1038"/>
-    <hyperlink ref="B61" r:id="rId54" display="#1037"/>
-    <hyperlink ref="B62" r:id="rId55" display="#1020"/>
-    <hyperlink ref="B63" r:id="rId56" display="#1032"/>
-    <hyperlink ref="B64" r:id="rId57" display="#1546"/>
-    <hyperlink ref="B65" r:id="rId58" display="#1027"/>
-    <hyperlink ref="B66" r:id="rId59" display="#1529"/>
-    <hyperlink ref="B68" r:id="rId60" display="#1527"/>
-    <hyperlink ref="B69" r:id="rId61" display="#558"/>
-    <hyperlink ref="B70" r:id="rId62" display="#1005"/>
-    <hyperlink ref="B71" r:id="rId63" display="#1020"/>
-    <hyperlink ref="B72" r:id="rId64" display="#993"/>
-    <hyperlink ref="B73" r:id="rId65" display="#1520"/>
-    <hyperlink ref="B74" r:id="rId66" display="#1519"/>
-    <hyperlink ref="B75" r:id="rId67" display="#969"/>
-    <hyperlink ref="B76" r:id="rId68" display="#1003"/>
-    <hyperlink ref="B77" r:id="rId69" display="#1015"/>
-    <hyperlink ref="B78" r:id="rId70" display="#1002"/>
-    <hyperlink ref="B79" r:id="rId71" display="#1471"/>
-    <hyperlink ref="B80" r:id="rId72" display="#1497"/>
-    <hyperlink ref="B81" r:id="rId73" display="#947"/>
-    <hyperlink ref="B82" r:id="rId74" display="#933"/>
-    <hyperlink ref="B83" r:id="rId75" display="#932"/>
-    <hyperlink ref="B84" r:id="rId76" display="#931"/>
-    <hyperlink ref="B85" r:id="rId77" display="#987"/>
-    <hyperlink ref="B86" r:id="rId78" display="#988"/>
-    <hyperlink ref="B87" r:id="rId79" display="#982"/>
-    <hyperlink ref="B88" r:id="rId80" display="#979"/>
-    <hyperlink ref="B89" r:id="rId81" display="#977"/>
-    <hyperlink ref="B90" r:id="rId82" display="#975"/>
-    <hyperlink ref="B91" r:id="rId83" display="#1445"/>
-    <hyperlink ref="B92" r:id="rId84" display="#1444"/>
-    <hyperlink ref="B93" r:id="rId85" display="#1427"/>
-    <hyperlink ref="B95" r:id="rId86" display="#23"/>
-    <hyperlink ref="B96" r:id="rId87" display="#22"/>
-    <hyperlink ref="B97" r:id="rId88" display="#18"/>
-    <hyperlink ref="B98" r:id="rId89" display="#1207"/>
-    <hyperlink ref="B99" r:id="rId90" display="#245"/>
+    <hyperlink ref="B6" r:id="rId3" display="#1171"/>
+    <hyperlink ref="B7" r:id="rId4" display="#1164"/>
+    <hyperlink ref="B8" r:id="rId5" display="#9"/>
+    <hyperlink ref="B9" r:id="rId6" display="#1163"/>
+    <hyperlink ref="B10" r:id="rId7" display="#1161"/>
+    <hyperlink ref="B11" r:id="rId8" display="#1690"/>
+    <hyperlink ref="B13" r:id="rId9" display="#1155"/>
+    <hyperlink ref="B14" r:id="rId10" display="#1150"/>
+    <hyperlink ref="B15" r:id="rId11" display="#1151"/>
+    <hyperlink ref="B16" r:id="rId12" display="#1200"/>
+    <hyperlink ref="B17" r:id="rId13" display="#1681"/>
+    <hyperlink ref="B18" r:id="rId14" display="#1142"/>
+    <hyperlink ref="B19" r:id="rId15" display="#8"/>
+    <hyperlink ref="B20" r:id="rId16" display="#1674"/>
+    <hyperlink ref="B21" r:id="rId17" display="#1672"/>
+    <hyperlink ref="B22" r:id="rId18" display="#1669"/>
+    <hyperlink ref="B23" r:id="rId19" display="#1670"/>
+    <hyperlink ref="B24" r:id="rId20" display="#1184"/>
+    <hyperlink ref="B25" r:id="rId21" display="#49"/>
+    <hyperlink ref="B26" r:id="rId22" display="#1140"/>
+    <hyperlink ref="B27" r:id="rId23" display="#1132"/>
+    <hyperlink ref="B29" r:id="rId24" display="#1125"/>
+    <hyperlink ref="B30" r:id="rId25" display="#1641"/>
+    <hyperlink ref="B31" r:id="rId26" display="#1124"/>
+    <hyperlink ref="B32" r:id="rId27" display="#1122"/>
+    <hyperlink ref="B33" r:id="rId28" display="#43"/>
+    <hyperlink ref="B34" r:id="rId29" display="#1622"/>
+    <hyperlink ref="B36" r:id="rId30" display="#38"/>
+    <hyperlink ref="B37" r:id="rId31" display="#1621"/>
+    <hyperlink ref="B38" r:id="rId32" display="#1616"/>
+    <hyperlink ref="B39" r:id="rId33" display="#37"/>
+    <hyperlink ref="B40" r:id="rId34" display="#36"/>
+    <hyperlink ref="B41" r:id="rId35" display="#1101"/>
+    <hyperlink ref="B42" r:id="rId36" display="#1099"/>
+    <hyperlink ref="B43" r:id="rId37" display="#1098"/>
+    <hyperlink ref="B44" r:id="rId38" display="#1617"/>
+    <hyperlink ref="B45" r:id="rId39" display="#1092"/>
+    <hyperlink ref="B46" r:id="rId40" display="#1128"/>
+    <hyperlink ref="B47" r:id="rId41" display="#1090"/>
+    <hyperlink ref="B48" r:id="rId42" display="#1608"/>
+    <hyperlink ref="B49" r:id="rId43" display="#35"/>
+    <hyperlink ref="B51" r:id="rId44" display="#1070"/>
+    <hyperlink ref="B52" r:id="rId45" display="#1592"/>
+    <hyperlink ref="B53" r:id="rId46" display="#1591"/>
+    <hyperlink ref="B54" r:id="rId47" display="#1578"/>
+    <hyperlink ref="B55" r:id="rId48" display="#41"/>
+    <hyperlink ref="B56" r:id="rId49" display="#42"/>
+    <hyperlink ref="B57" r:id="rId50" display="#1566"/>
+    <hyperlink ref="B58" r:id="rId51" display="#1565"/>
+    <hyperlink ref="B59" r:id="rId52" display="#1046"/>
+    <hyperlink ref="B60" r:id="rId53" display="#1559"/>
+    <hyperlink ref="B61" r:id="rId54" display="#1038"/>
+    <hyperlink ref="B62" r:id="rId55" display="#1037"/>
+    <hyperlink ref="B63" r:id="rId56" display="#1020"/>
+    <hyperlink ref="B64" r:id="rId57" display="#1032"/>
+    <hyperlink ref="B65" r:id="rId58" display="#1546"/>
+    <hyperlink ref="B66" r:id="rId59" display="#1027"/>
+    <hyperlink ref="B67" r:id="rId60" display="#1529"/>
+    <hyperlink ref="B69" r:id="rId61" display="#1527"/>
+    <hyperlink ref="B70" r:id="rId62" display="#558"/>
+    <hyperlink ref="B71" r:id="rId63" display="#1005"/>
+    <hyperlink ref="B72" r:id="rId64" display="#1020"/>
+    <hyperlink ref="B73" r:id="rId65" display="#993"/>
+    <hyperlink ref="B74" r:id="rId66" display="#1520"/>
+    <hyperlink ref="B75" r:id="rId67" display="#1519"/>
+    <hyperlink ref="B76" r:id="rId68" display="#969"/>
+    <hyperlink ref="B77" r:id="rId69" display="#1003"/>
+    <hyperlink ref="B78" r:id="rId70" display="#1015"/>
+    <hyperlink ref="B79" r:id="rId71" display="#1002"/>
+    <hyperlink ref="B80" r:id="rId72" display="#1471"/>
+    <hyperlink ref="B81" r:id="rId73" display="#1497"/>
+    <hyperlink ref="B82" r:id="rId74" display="#947"/>
+    <hyperlink ref="B83" r:id="rId75" display="#933"/>
+    <hyperlink ref="B84" r:id="rId76" display="#932"/>
+    <hyperlink ref="B85" r:id="rId77" display="#931"/>
+    <hyperlink ref="B86" r:id="rId78" display="#987"/>
+    <hyperlink ref="B87" r:id="rId79" display="#988"/>
+    <hyperlink ref="B88" r:id="rId80" display="#982"/>
+    <hyperlink ref="B89" r:id="rId81" display="#979"/>
+    <hyperlink ref="B90" r:id="rId82" display="#977"/>
+    <hyperlink ref="B91" r:id="rId83" display="#975"/>
+    <hyperlink ref="B92" r:id="rId84" display="#1445"/>
+    <hyperlink ref="B93" r:id="rId85" display="#1444"/>
+    <hyperlink ref="B94" r:id="rId86" display="#1427"/>
+    <hyperlink ref="B96" r:id="rId87" display="#23"/>
+    <hyperlink ref="B97" r:id="rId88" display="#22"/>
+    <hyperlink ref="B98" r:id="rId89" display="#18"/>
+    <hyperlink ref="B99" r:id="rId90" display="#1207"/>
+    <hyperlink ref="B100" r:id="rId91" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -3484,7 +3514,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId91"/>
+  <drawing r:id="rId92"/>
 </worksheet>
 </file>
 
@@ -3517,10 +3547,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -3529,10 +3559,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added omt plugin issue #11
</commit_message>
<xml_diff>
--- a/tickets/OmegaT_issues_nopw.xlsx
+++ b/tickets/OmegaT_issues_nopw.xlsx
@@ -13,7 +13,7 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$100</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$101</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"Devs"</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="238">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -123,15 +123,24 @@
     <t xml:space="preserve">WIP</t>
   </si>
   <si>
+    <t xml:space="preserve">#11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plugin-omt-package</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoClassDefFoundError when packing project in OmegaT 6.1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open!!</t>
+  </si>
+  <si>
     <t xml:space="preserve">#1309</t>
   </si>
   <si>
     <t xml:space="preserve">XML filter does not extract resname if unit contains HTML block-level tags</t>
   </si>
   <si>
-    <t xml:space="preserve">Open!!</t>
-  </si>
-  <si>
     <t xml:space="preserve">#1176</t>
   </si>
   <si>
@@ -160,9 +169,6 @@
   </si>
   <si>
     <t xml:space="preserve">#9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plugin-omt-package</t>
   </si>
   <si>
     <t xml:space="preserve">Add property in config to remove mappings (to pack as offline project)</t>
@@ -1369,7 +1375,7 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ102"/>
+  <dimension ref="A1:AMJ103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1432,22 +1438,22 @@
     </row>
     <row r="4" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
-        <v>45069</v>
+        <v>45094</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
@@ -1458,19 +1464,19 @@
         <v>45069</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
@@ -1478,7 +1484,7 @@
     </row>
     <row r="6" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
-        <v>45064</v>
+        <v>45069</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>36</v>
@@ -1501,7 +1507,7 @@
     </row>
     <row r="7" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
-        <v>45049</v>
+        <v>45064</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>39</v>
@@ -1529,17 +1535,17 @@
       <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
@@ -1547,22 +1553,22 @@
     </row>
     <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
-        <v>45044</v>
+        <v>45049</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="F9" s="9" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
@@ -1570,7 +1576,7 @@
     </row>
     <row r="10" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="n">
-        <v>45040</v>
+        <v>45044</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>48</v>
@@ -1585,7 +1591,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
@@ -1593,7 +1599,7 @@
     </row>
     <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>50</v>
@@ -1605,10 +1611,10 @@
         <v>51</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
@@ -1616,16 +1622,22 @@
     </row>
     <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>53</v>
       </c>
+      <c r="E12" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="F12" s="9" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
@@ -1633,19 +1645,13 @@
     </row>
     <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B13" s="11" t="s">
+        <v>44996</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>38</v>
@@ -1656,7 +1662,7 @@
     </row>
     <row r="14" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>56</v>
@@ -1671,7 +1677,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
@@ -1694,7 +1700,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
@@ -1702,13 +1708,13 @@
     </row>
     <row r="16" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>61</v>
@@ -1717,7 +1723,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
@@ -1725,22 +1731,22 @@
     </row>
     <row r="17" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="9" t="s">
+      <c r="E17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
@@ -1748,7 +1754,7 @@
     </row>
     <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="n">
-        <v>44972</v>
+        <v>44981</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>65</v>
@@ -1760,33 +1766,33 @@
         <v>66</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
       <c r="AMJ18" s="0"/>
     </row>
-    <row r="19" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B19" s="14" t="s">
+    <row r="19" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>38</v>
+      <c r="E19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
@@ -1794,22 +1800,22 @@
     </row>
     <row r="20" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>69</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
@@ -1817,22 +1823,22 @@
     </row>
     <row r="21" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="E21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="AMH21" s="0"/>
       <c r="AMI21" s="0"/>
@@ -1840,7 +1846,7 @@
     </row>
     <row r="22" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>74</v>
@@ -1852,10 +1858,10 @@
         <v>75</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
@@ -1875,10 +1881,10 @@
         <v>77</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>78</v>
+        <v>33</v>
       </c>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
@@ -1886,22 +1892,22 @@
     </row>
     <row r="24" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="n">
-        <v>44949</v>
+        <v>44952</v>
       </c>
       <c r="B24" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="12" t="s">
+      <c r="E24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
@@ -1909,22 +1915,22 @@
     </row>
     <row r="25" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="n">
-        <v>44948</v>
+        <v>44949</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>82</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="AMH25" s="0"/>
       <c r="AMI25" s="0"/>
@@ -1932,125 +1938,125 @@
     </row>
     <row r="26" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>83</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>84</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
       <c r="AMJ26" s="0"/>
     </row>
-    <row r="27" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B27" s="16" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>87</v>
-      </c>
       <c r="E27" s="12" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+    <row r="28" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>29</v>
+      <c r="C28" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="5" t="s">
+    <row r="29" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>38</v>
+      <c r="F29" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B30" s="14" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="12" t="s">
+      <c r="C30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>38</v>
+      <c r="E30" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B31" s="17" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>32</v>
+      <c r="E31" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>41</v>
       </c>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
@@ -2058,7 +2064,7 @@
     </row>
     <row r="32" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>95</v>
@@ -2070,112 +2076,115 @@
         <v>96</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B33" s="18" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="E33" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>78</v>
-      </c>
+      <c r="AMH33" s="0"/>
+      <c r="AMI33" s="0"/>
+      <c r="AMJ33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B34" s="17" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>102</v>
       </c>
       <c r="E34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="13" t="n">
+        <v>373466</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="n">
-        <v>44743</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>103</v>
-      </c>
       <c r="F35" s="5" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>104</v>
+        <v>44743</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E36" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="F36" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B37" s="20" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B37" s="19" t="s">
         <v>106</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>107</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>108</v>
@@ -2187,90 +2196,90 @@
         <v>109</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B39" s="21" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B39" s="20" t="s">
         <v>110</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>111</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="n">
-        <v>44659</v>
+        <v>44695</v>
       </c>
       <c r="B40" s="21" t="s">
         <v>112</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B41" s="20" t="s">
+        <v>44659</v>
+      </c>
+      <c r="B41" s="21" t="s">
         <v>114</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B42" s="17" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="E42" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,15 +2296,15 @@
         <v>120</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>121</v>
@@ -2307,15 +2316,15 @@
         <v>122</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="13" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>123</v>
@@ -2327,57 +2336,57 @@
         <v>124</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>125</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>126</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>127</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>128</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B48" s="20" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B48" s="17" t="s">
         <v>129</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -2387,60 +2396,60 @@
         <v>130</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="13" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B49" s="17" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>131</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>132</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="13" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="13" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B51" s="17" t="s">
+      <c r="C50" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C51" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="5" t="s">
+      <c r="E50" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="13" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>136</v>
@@ -2452,10 +2461,10 @@
         <v>137</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>138</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,24 +2472,24 @@
         <v>44460</v>
       </c>
       <c r="B53" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="13" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>141</v>
@@ -2495,72 +2504,72 @@
         <v>23</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="13" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>143</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>144</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="13" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B56" s="21" t="s">
+        <v>44326</v>
+      </c>
+      <c r="B56" s="17" t="s">
         <v>145</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>146</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="13" t="n">
         <v>44325</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="21" t="s">
         <v>147</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>148</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="13" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>149</v>
@@ -2572,15 +2581,15 @@
         <v>150</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="13" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B59" s="17" t="s">
         <v>151</v>
@@ -2592,37 +2601,37 @@
         <v>152</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>153</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B60" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" s="5" t="s">
+      <c r="E60" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F60" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="13" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B61" s="17" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>156</v>
       </c>
       <c r="C61" s="5" t="s">
@@ -2632,15 +2641,15 @@
         <v>157</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="13" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B62" s="17" t="s">
         <v>158</v>
@@ -2652,57 +2661,57 @@
         <v>159</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="22" t="n">
+      <c r="A63" s="13" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="22" t="n">
         <v>44231</v>
       </c>
-      <c r="B63" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="E63" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="13" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="5" t="s">
+      <c r="C64" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E64" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F64" s="24" t="s">
         <v>163</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="13" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B65" s="20" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B65" s="17" t="s">
         <v>164</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2712,17 +2721,17 @@
         <v>165</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="13" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B66" s="17" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B66" s="20" t="s">
         <v>166</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -2732,10 +2741,10 @@
         <v>167</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,40 +2761,40 @@
         <v>169</v>
       </c>
       <c r="E67" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="13" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E68" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F67" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="13" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>38</v>
+      <c r="F68" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="13" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B70" s="17" t="s">
         <v>172</v>
@@ -2794,158 +2803,158 @@
         <v>7</v>
       </c>
       <c r="D70" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="13" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="22" t="n">
+      <c r="E71" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="22" t="n">
         <v>44146</v>
       </c>
-      <c r="B71" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="C71" s="24" t="s">
+      <c r="B72" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D71" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="E71" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F71" s="24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="13" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="E72" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>38</v>
+      <c r="E72" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="13" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>178</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="22" t="n">
+      <c r="A74" s="13" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B74" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D74" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="22" t="n">
         <v>44095</v>
       </c>
-      <c r="B74" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="C74" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="E74" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F74" s="24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="13" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="C75" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" s="5" t="s">
+      <c r="C75" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="24" t="s">
         <v>182</v>
       </c>
-      <c r="E75" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>38</v>
+      <c r="E75" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="13" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B76" s="17" t="s">
         <v>183</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>184</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>138</v>
+        <v>41</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="13" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B77" s="17" t="s">
         <v>185</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>186</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>78</v>
+        <v>140</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="13" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>187</v>
@@ -2957,15 +2966,15 @@
         <v>188</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="13" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>189</v>
@@ -2977,15 +2986,15 @@
         <v>190</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B80" s="17" t="s">
         <v>191</v>
@@ -2997,15 +3006,15 @@
         <v>192</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="13" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>193</v>
@@ -3017,35 +3026,35 @@
         <v>194</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="13" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B82" s="17" t="s">
         <v>195</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>196</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="13" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B83" s="17" t="s">
         <v>197</v>
@@ -3057,15 +3066,15 @@
         <v>198</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="13" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B84" s="17" t="s">
         <v>199</v>
@@ -3077,15 +3086,15 @@
         <v>200</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="13" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B85" s="17" t="s">
         <v>201</v>
@@ -3097,35 +3106,35 @@
         <v>202</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="13" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>203</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>204</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="13" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B87" s="17" t="s">
         <v>205</v>
@@ -3137,15 +3146,15 @@
         <v>206</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="13" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B88" s="17" t="s">
         <v>207</v>
@@ -3157,15 +3166,15 @@
         <v>208</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="13" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B89" s="17" t="s">
         <v>209</v>
@@ -3177,10 +3186,10 @@
         <v>210</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,15 +3206,15 @@
         <v>212</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="13" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B91" s="17" t="s">
         <v>213</v>
@@ -3217,15 +3226,15 @@
         <v>214</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="13" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B92" s="17" t="s">
         <v>215</v>
@@ -3237,10 +3246,10 @@
         <v>216</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3260,14 +3269,14 @@
         <v>23</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="13" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B94" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B94" s="17" t="s">
         <v>219</v>
       </c>
       <c r="C94" s="5" t="s">
@@ -3280,32 +3289,32 @@
         <v>23</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="13" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B96" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="13" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B95" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C96" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D96" s="5" t="s">
+      <c r="C95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="E96" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>71</v>
+      <c r="E95" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3316,61 +3325,61 @@
         <v>223</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>224</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="13" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B98" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D98" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="C98" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D98" s="5" t="s">
+      <c r="E98" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F98" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="13" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B99" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B99" s="25" t="s">
         <v>228</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>229</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="13" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>230</v>
@@ -3382,19 +3391,39 @@
         <v>231</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="102" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMH102" s="0"/>
-      <c r="AMI102" s="0"/>
-      <c r="AMJ102" s="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="13" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="103" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMH103" s="0"/>
+      <c r="AMI103" s="0"/>
+      <c r="AMJ103" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F100">
+  <autoFilter ref="A1:F101">
     <filterColumn colId="5">
       <filters>
         <filter val="Fixed?"/>
@@ -3415,97 +3444,98 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="#1309"/>
-    <hyperlink ref="B5" r:id="rId2" display="#1176"/>
-    <hyperlink ref="B6" r:id="rId3" display="#1171"/>
-    <hyperlink ref="B7" r:id="rId4" display="#1164"/>
-    <hyperlink ref="B8" r:id="rId5" display="#9"/>
-    <hyperlink ref="B9" r:id="rId6" display="#1163"/>
-    <hyperlink ref="B10" r:id="rId7" display="#1161"/>
-    <hyperlink ref="B11" r:id="rId8" display="#1690"/>
-    <hyperlink ref="B13" r:id="rId9" display="#1155"/>
-    <hyperlink ref="B14" r:id="rId10" display="#1150"/>
-    <hyperlink ref="B15" r:id="rId11" display="#1151"/>
-    <hyperlink ref="B16" r:id="rId12" display="#1200"/>
-    <hyperlink ref="B17" r:id="rId13" display="#1681"/>
-    <hyperlink ref="B18" r:id="rId14" display="#1142"/>
-    <hyperlink ref="B19" r:id="rId15" display="#8"/>
-    <hyperlink ref="B20" r:id="rId16" display="#1674"/>
-    <hyperlink ref="B21" r:id="rId17" display="#1672"/>
-    <hyperlink ref="B22" r:id="rId18" display="#1669"/>
-    <hyperlink ref="B23" r:id="rId19" display="#1670"/>
-    <hyperlink ref="B24" r:id="rId20" display="#1184"/>
-    <hyperlink ref="B25" r:id="rId21" display="#49"/>
-    <hyperlink ref="B26" r:id="rId22" display="#1140"/>
-    <hyperlink ref="B27" r:id="rId23" display="#1132"/>
-    <hyperlink ref="B29" r:id="rId24" display="#1125"/>
-    <hyperlink ref="B30" r:id="rId25" display="#1641"/>
-    <hyperlink ref="B31" r:id="rId26" display="#1124"/>
-    <hyperlink ref="B32" r:id="rId27" display="#1122"/>
-    <hyperlink ref="B33" r:id="rId28" display="#43"/>
-    <hyperlink ref="B34" r:id="rId29" display="#1622"/>
-    <hyperlink ref="B36" r:id="rId30" display="#38"/>
-    <hyperlink ref="B37" r:id="rId31" display="#1621"/>
-    <hyperlink ref="B38" r:id="rId32" display="#1616"/>
-    <hyperlink ref="B39" r:id="rId33" display="#37"/>
-    <hyperlink ref="B40" r:id="rId34" display="#36"/>
-    <hyperlink ref="B41" r:id="rId35" display="#1101"/>
-    <hyperlink ref="B42" r:id="rId36" display="#1099"/>
-    <hyperlink ref="B43" r:id="rId37" display="#1098"/>
-    <hyperlink ref="B44" r:id="rId38" display="#1617"/>
-    <hyperlink ref="B45" r:id="rId39" display="#1092"/>
-    <hyperlink ref="B46" r:id="rId40" display="#1128"/>
-    <hyperlink ref="B47" r:id="rId41" display="#1090"/>
-    <hyperlink ref="B48" r:id="rId42" display="#1608"/>
-    <hyperlink ref="B49" r:id="rId43" display="#35"/>
-    <hyperlink ref="B51" r:id="rId44" display="#1070"/>
-    <hyperlink ref="B52" r:id="rId45" display="#1592"/>
-    <hyperlink ref="B53" r:id="rId46" display="#1591"/>
-    <hyperlink ref="B54" r:id="rId47" display="#1578"/>
-    <hyperlink ref="B55" r:id="rId48" display="#41"/>
-    <hyperlink ref="B56" r:id="rId49" display="#42"/>
-    <hyperlink ref="B57" r:id="rId50" display="#1566"/>
-    <hyperlink ref="B58" r:id="rId51" display="#1565"/>
-    <hyperlink ref="B59" r:id="rId52" display="#1046"/>
-    <hyperlink ref="B60" r:id="rId53" display="#1559"/>
-    <hyperlink ref="B61" r:id="rId54" display="#1038"/>
-    <hyperlink ref="B62" r:id="rId55" display="#1037"/>
-    <hyperlink ref="B63" r:id="rId56" display="#1020"/>
-    <hyperlink ref="B64" r:id="rId57" display="#1032"/>
-    <hyperlink ref="B65" r:id="rId58" display="#1546"/>
-    <hyperlink ref="B66" r:id="rId59" display="#1027"/>
-    <hyperlink ref="B67" r:id="rId60" display="#1529"/>
-    <hyperlink ref="B69" r:id="rId61" display="#1527"/>
-    <hyperlink ref="B70" r:id="rId62" display="#558"/>
-    <hyperlink ref="B71" r:id="rId63" display="#1005"/>
-    <hyperlink ref="B72" r:id="rId64" display="#1020"/>
-    <hyperlink ref="B73" r:id="rId65" display="#993"/>
-    <hyperlink ref="B74" r:id="rId66" display="#1520"/>
-    <hyperlink ref="B75" r:id="rId67" display="#1519"/>
-    <hyperlink ref="B76" r:id="rId68" display="#969"/>
-    <hyperlink ref="B77" r:id="rId69" display="#1003"/>
-    <hyperlink ref="B78" r:id="rId70" display="#1015"/>
-    <hyperlink ref="B79" r:id="rId71" display="#1002"/>
-    <hyperlink ref="B80" r:id="rId72" display="#1471"/>
-    <hyperlink ref="B81" r:id="rId73" display="#1497"/>
-    <hyperlink ref="B82" r:id="rId74" display="#947"/>
-    <hyperlink ref="B83" r:id="rId75" display="#933"/>
-    <hyperlink ref="B84" r:id="rId76" display="#932"/>
-    <hyperlink ref="B85" r:id="rId77" display="#931"/>
-    <hyperlink ref="B86" r:id="rId78" display="#987"/>
-    <hyperlink ref="B87" r:id="rId79" display="#988"/>
-    <hyperlink ref="B88" r:id="rId80" display="#982"/>
-    <hyperlink ref="B89" r:id="rId81" display="#979"/>
-    <hyperlink ref="B90" r:id="rId82" display="#977"/>
-    <hyperlink ref="B91" r:id="rId83" display="#975"/>
-    <hyperlink ref="B92" r:id="rId84" display="#1445"/>
-    <hyperlink ref="B93" r:id="rId85" display="#1444"/>
-    <hyperlink ref="B94" r:id="rId86" display="#1427"/>
-    <hyperlink ref="B96" r:id="rId87" display="#23"/>
-    <hyperlink ref="B97" r:id="rId88" display="#22"/>
-    <hyperlink ref="B98" r:id="rId89" display="#18"/>
-    <hyperlink ref="B99" r:id="rId90" display="#1207"/>
-    <hyperlink ref="B100" r:id="rId91" display="#245"/>
+    <hyperlink ref="B4" r:id="rId1" display="#11"/>
+    <hyperlink ref="B5" r:id="rId2" display="#1309"/>
+    <hyperlink ref="B6" r:id="rId3" display="#1176"/>
+    <hyperlink ref="B7" r:id="rId4" display="#1171"/>
+    <hyperlink ref="B8" r:id="rId5" display="#1164"/>
+    <hyperlink ref="B9" r:id="rId6" display="#9"/>
+    <hyperlink ref="B10" r:id="rId7" display="#1163"/>
+    <hyperlink ref="B11" r:id="rId8" display="#1161"/>
+    <hyperlink ref="B12" r:id="rId9" display="#1690"/>
+    <hyperlink ref="B14" r:id="rId10" display="#1155"/>
+    <hyperlink ref="B15" r:id="rId11" display="#1150"/>
+    <hyperlink ref="B16" r:id="rId12" display="#1151"/>
+    <hyperlink ref="B17" r:id="rId13" display="#1200"/>
+    <hyperlink ref="B18" r:id="rId14" display="#1681"/>
+    <hyperlink ref="B19" r:id="rId15" display="#1142"/>
+    <hyperlink ref="B20" r:id="rId16" display="#8"/>
+    <hyperlink ref="B21" r:id="rId17" display="#1674"/>
+    <hyperlink ref="B22" r:id="rId18" display="#1672"/>
+    <hyperlink ref="B23" r:id="rId19" display="#1669"/>
+    <hyperlink ref="B24" r:id="rId20" display="#1670"/>
+    <hyperlink ref="B25" r:id="rId21" display="#1184"/>
+    <hyperlink ref="B26" r:id="rId22" display="#49"/>
+    <hyperlink ref="B27" r:id="rId23" display="#1140"/>
+    <hyperlink ref="B28" r:id="rId24" display="#1132"/>
+    <hyperlink ref="B30" r:id="rId25" display="#1125"/>
+    <hyperlink ref="B31" r:id="rId26" display="#1641"/>
+    <hyperlink ref="B32" r:id="rId27" display="#1124"/>
+    <hyperlink ref="B33" r:id="rId28" display="#1122"/>
+    <hyperlink ref="B34" r:id="rId29" display="#43"/>
+    <hyperlink ref="B35" r:id="rId30" display="#1622"/>
+    <hyperlink ref="B37" r:id="rId31" display="#38"/>
+    <hyperlink ref="B38" r:id="rId32" display="#1621"/>
+    <hyperlink ref="B39" r:id="rId33" display="#1616"/>
+    <hyperlink ref="B40" r:id="rId34" display="#37"/>
+    <hyperlink ref="B41" r:id="rId35" display="#36"/>
+    <hyperlink ref="B42" r:id="rId36" display="#1101"/>
+    <hyperlink ref="B43" r:id="rId37" display="#1099"/>
+    <hyperlink ref="B44" r:id="rId38" display="#1098"/>
+    <hyperlink ref="B45" r:id="rId39" display="#1617"/>
+    <hyperlink ref="B46" r:id="rId40" display="#1092"/>
+    <hyperlink ref="B47" r:id="rId41" display="#1128"/>
+    <hyperlink ref="B48" r:id="rId42" display="#1090"/>
+    <hyperlink ref="B49" r:id="rId43" display="#1608"/>
+    <hyperlink ref="B50" r:id="rId44" display="#35"/>
+    <hyperlink ref="B52" r:id="rId45" display="#1070"/>
+    <hyperlink ref="B53" r:id="rId46" display="#1592"/>
+    <hyperlink ref="B54" r:id="rId47" display="#1591"/>
+    <hyperlink ref="B55" r:id="rId48" display="#1578"/>
+    <hyperlink ref="B56" r:id="rId49" display="#41"/>
+    <hyperlink ref="B57" r:id="rId50" display="#42"/>
+    <hyperlink ref="B58" r:id="rId51" display="#1566"/>
+    <hyperlink ref="B59" r:id="rId52" display="#1565"/>
+    <hyperlink ref="B60" r:id="rId53" display="#1046"/>
+    <hyperlink ref="B61" r:id="rId54" display="#1559"/>
+    <hyperlink ref="B62" r:id="rId55" display="#1038"/>
+    <hyperlink ref="B63" r:id="rId56" display="#1037"/>
+    <hyperlink ref="B64" r:id="rId57" display="#1020"/>
+    <hyperlink ref="B65" r:id="rId58" display="#1032"/>
+    <hyperlink ref="B66" r:id="rId59" display="#1546"/>
+    <hyperlink ref="B67" r:id="rId60" display="#1027"/>
+    <hyperlink ref="B68" r:id="rId61" display="#1529"/>
+    <hyperlink ref="B70" r:id="rId62" display="#1527"/>
+    <hyperlink ref="B71" r:id="rId63" display="#558"/>
+    <hyperlink ref="B72" r:id="rId64" display="#1005"/>
+    <hyperlink ref="B73" r:id="rId65" display="#1020"/>
+    <hyperlink ref="B74" r:id="rId66" display="#993"/>
+    <hyperlink ref="B75" r:id="rId67" display="#1520"/>
+    <hyperlink ref="B76" r:id="rId68" display="#1519"/>
+    <hyperlink ref="B77" r:id="rId69" display="#969"/>
+    <hyperlink ref="B78" r:id="rId70" display="#1003"/>
+    <hyperlink ref="B79" r:id="rId71" display="#1015"/>
+    <hyperlink ref="B80" r:id="rId72" display="#1002"/>
+    <hyperlink ref="B81" r:id="rId73" display="#1471"/>
+    <hyperlink ref="B82" r:id="rId74" display="#1497"/>
+    <hyperlink ref="B83" r:id="rId75" display="#947"/>
+    <hyperlink ref="B84" r:id="rId76" display="#933"/>
+    <hyperlink ref="B85" r:id="rId77" display="#932"/>
+    <hyperlink ref="B86" r:id="rId78" display="#931"/>
+    <hyperlink ref="B87" r:id="rId79" display="#987"/>
+    <hyperlink ref="B88" r:id="rId80" display="#988"/>
+    <hyperlink ref="B89" r:id="rId81" display="#982"/>
+    <hyperlink ref="B90" r:id="rId82" display="#979"/>
+    <hyperlink ref="B91" r:id="rId83" display="#977"/>
+    <hyperlink ref="B92" r:id="rId84" display="#975"/>
+    <hyperlink ref="B93" r:id="rId85" display="#1445"/>
+    <hyperlink ref="B94" r:id="rId86" display="#1444"/>
+    <hyperlink ref="B95" r:id="rId87" display="#1427"/>
+    <hyperlink ref="B97" r:id="rId88" display="#23"/>
+    <hyperlink ref="B98" r:id="rId89" display="#22"/>
+    <hyperlink ref="B99" r:id="rId90" display="#18"/>
+    <hyperlink ref="B100" r:id="rId91" display="#1207"/>
+    <hyperlink ref="B101" r:id="rId92" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -3514,7 +3544,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId92"/>
+  <drawing r:id="rId93"/>
 </worksheet>
 </file>
 
@@ -3547,10 +3577,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -3559,10 +3589,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added OmegaT ticket #1185 and updated a few others
</commit_message>
<xml_diff>
--- a/tickets/OmegaT_issues_nopw.xlsx
+++ b/tickets/OmegaT_issues_nopw.xlsx
@@ -13,7 +13,7 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$101</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$102</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"Devs"</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="240">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -123,6 +123,15 @@
     <t xml:space="preserve">WIP</t>
   </si>
   <si>
+    <t xml:space="preserve">#1185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saving does not register pre-translation in new projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open!!</t>
+  </si>
+  <si>
     <t xml:space="preserve">#11</t>
   </si>
   <si>
@@ -132,7 +141,7 @@
     <t xml:space="preserve">NoClassDefFoundError when packing project in OmegaT 6.1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Open!!</t>
+    <t xml:space="preserve">Solved</t>
   </si>
   <si>
     <t xml:space="preserve">#1309</t>
@@ -145,9 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">The COMPILE event is fired *after* the target commit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solved</t>
   </si>
   <si>
     <t xml:space="preserve">#1171</t>
@@ -1375,7 +1381,7 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ103"/>
+  <dimension ref="A1:AMJ104"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1438,22 +1444,22 @@
     </row>
     <row r="4" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
-        <v>45094</v>
+        <v>45104</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>32</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
@@ -1461,13 +1467,13 @@
     </row>
     <row r="5" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="n">
-        <v>45069</v>
+        <v>45094</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>35</v>
@@ -1476,7 +1482,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AMH5" s="0"/>
       <c r="AMI5" s="0"/>
@@ -1487,19 +1493,19 @@
         <v>45069</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
@@ -1507,7 +1513,7 @@
     </row>
     <row r="7" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
-        <v>45064</v>
+        <v>45069</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>39</v>
@@ -1522,7 +1528,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AMH7" s="0"/>
       <c r="AMI7" s="0"/>
@@ -1530,22 +1536,22 @@
     </row>
     <row r="8" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
-        <v>45049</v>
+        <v>45064</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
@@ -1556,19 +1562,19 @@
         <v>45049</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="E9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
@@ -1576,22 +1582,22 @@
     </row>
     <row r="10" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="n">
-        <v>45044</v>
+        <v>45049</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="F10" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
@@ -1599,7 +1605,7 @@
     </row>
     <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="n">
-        <v>45040</v>
+        <v>45044</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>50</v>
@@ -1614,7 +1620,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
@@ -1622,7 +1628,7 @@
     </row>
     <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>52</v>
@@ -1634,10 +1640,10 @@
         <v>53</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
@@ -1645,16 +1651,22 @@
     </row>
     <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>54</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>55</v>
       </c>
+      <c r="E13" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="F13" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
@@ -1662,22 +1674,16 @@
     </row>
     <row r="14" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B14" s="11" t="s">
+        <v>44996</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="F14" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
@@ -1685,7 +1691,7 @@
     </row>
     <row r="15" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>58</v>
@@ -1700,7 +1706,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
@@ -1723,7 +1729,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
@@ -1731,13 +1737,13 @@
     </row>
     <row r="17" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>62</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>63</v>
@@ -1746,7 +1752,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
@@ -1754,22 +1760,22 @@
     </row>
     <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="9" t="s">
+      <c r="E18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
@@ -1777,7 +1783,7 @@
     </row>
     <row r="19" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="n">
-        <v>44972</v>
+        <v>44981</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>67</v>
@@ -1789,33 +1795,33 @@
         <v>68</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
       <c r="AMJ19" s="0"/>
     </row>
-    <row r="20" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B20" s="14" t="s">
+    <row r="20" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="10" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="12" t="s">
+      <c r="C20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>41</v>
+      <c r="E20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
@@ -1823,22 +1829,22 @@
     </row>
     <row r="21" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="AMH21" s="0"/>
       <c r="AMI21" s="0"/>
@@ -1846,22 +1852,22 @@
     </row>
     <row r="22" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B22" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="12" t="s">
+      <c r="E22" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
@@ -1869,7 +1875,7 @@
     </row>
     <row r="23" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>76</v>
@@ -1881,10 +1887,10 @@
         <v>77</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
@@ -1904,10 +1910,10 @@
         <v>79</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
@@ -1915,22 +1921,22 @@
     </row>
     <row r="25" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="n">
-        <v>44949</v>
+        <v>44952</v>
       </c>
       <c r="B25" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="E25" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="AMH25" s="0"/>
       <c r="AMI25" s="0"/>
@@ -1938,22 +1944,22 @@
     </row>
     <row r="26" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="n">
-        <v>44948</v>
+        <v>44949</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>83</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>84</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
@@ -1961,125 +1967,125 @@
     </row>
     <row r="27" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>85</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>86</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
       <c r="AMJ27" s="0"/>
     </row>
-    <row r="28" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B28" s="16" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>89</v>
-      </c>
       <c r="E28" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
+    <row r="29" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B29" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>29</v>
+      <c r="C29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="5" t="s">
+    <row r="30" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>41</v>
+      <c r="F30" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B31" s="14" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="12" t="s">
+      <c r="C31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>41</v>
+      <c r="E31" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
-    <row r="32" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B32" s="17" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B32" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="5" t="s">
+      <c r="C32" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>33</v>
+      <c r="E32" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
@@ -2087,7 +2093,7 @@
     </row>
     <row r="33" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>97</v>
@@ -2099,112 +2105,115 @@
         <v>98</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="AMH33" s="0"/>
       <c r="AMI33" s="0"/>
       <c r="AMJ33" s="0"/>
     </row>
-    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B34" s="18" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="E34" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="AMH34" s="0"/>
+      <c r="AMI34" s="0"/>
+      <c r="AMJ34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B35" s="17" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>104</v>
       </c>
       <c r="E35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="13" t="n">
+        <v>373466</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13" t="n">
-        <v>44743</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="F36" s="5" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>106</v>
+        <v>44743</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="F37" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B38" s="20" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B38" s="19" t="s">
         <v>108</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>109</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>110</v>
@@ -2216,90 +2225,90 @@
         <v>111</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B40" s="21" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B40" s="20" t="s">
         <v>112</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="n">
-        <v>44659</v>
+        <v>44695</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>114</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B42" s="20" t="s">
+        <v>44659</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>116</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>117</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="13" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B43" s="17" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="5" t="s">
+      <c r="E43" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2316,15 +2325,15 @@
         <v>122</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="13" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>123</v>
@@ -2336,15 +2345,15 @@
         <v>124</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>125</v>
@@ -2356,57 +2365,57 @@
         <v>126</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>127</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>128</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>129</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>130</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="13" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B49" s="20" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B49" s="17" t="s">
         <v>131</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -2416,60 +2425,60 @@
         <v>132</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="13" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B50" s="17" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B50" s="20" t="s">
         <v>133</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="13" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B51" s="17" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="13" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B52" s="17" t="s">
+      <c r="C51" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="E51" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="13" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B53" s="17" t="s">
         <v>138</v>
@@ -2481,10 +2490,10 @@
         <v>139</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>140</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,24 +2501,24 @@
         <v>44460</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="E54" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="13" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B55" s="17" t="s">
         <v>143</v>
@@ -2524,72 +2533,72 @@
         <v>23</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="13" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>145</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>146</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="13" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B57" s="21" t="s">
+        <v>44326</v>
+      </c>
+      <c r="B57" s="17" t="s">
         <v>147</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>148</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="13" t="n">
         <v>44325</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="21" t="s">
         <v>149</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>150</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="13" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B59" s="17" t="s">
         <v>151</v>
@@ -2601,15 +2610,15 @@
         <v>152</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B60" s="17" t="s">
         <v>153</v>
@@ -2621,37 +2630,37 @@
         <v>154</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="13" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B61" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="5" t="s">
+      <c r="E61" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>157</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="13" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B62" s="17" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>158</v>
       </c>
       <c r="C62" s="5" t="s">
@@ -2661,15 +2670,15 @@
         <v>159</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="13" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B63" s="17" t="s">
         <v>160</v>
@@ -2681,57 +2690,57 @@
         <v>161</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="22" t="n">
+      <c r="A64" s="13" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="22" t="n">
         <v>44231</v>
       </c>
-      <c r="B64" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="24" t="s">
-        <v>107</v>
-      </c>
-      <c r="E64" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="13" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="5" t="s">
+      <c r="C65" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F65" s="24" t="s">
         <v>165</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="13" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B66" s="20" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B66" s="17" t="s">
         <v>166</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -2741,17 +2750,17 @@
         <v>167</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="13" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B67" s="17" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B67" s="20" t="s">
         <v>168</v>
       </c>
       <c r="C67" s="5" t="s">
@@ -2761,10 +2770,10 @@
         <v>169</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2781,40 +2790,40 @@
         <v>171</v>
       </c>
       <c r="E68" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="13" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F68" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="13" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>41</v>
+      <c r="F69" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="13" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B71" s="17" t="s">
         <v>174</v>
@@ -2823,158 +2832,158 @@
         <v>7</v>
       </c>
       <c r="D71" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="13" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E71" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="22" t="n">
+      <c r="E72" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="22" t="n">
         <v>44146</v>
       </c>
-      <c r="B72" s="23" t="s">
-        <v>175</v>
-      </c>
-      <c r="C72" s="24" t="s">
+      <c r="B73" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="C73" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D72" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="E72" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F72" s="24" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="13" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="24" t="s">
         <v>178</v>
       </c>
-      <c r="E73" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>41</v>
+      <c r="E73" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="13" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>180</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="22" t="n">
+      <c r="A75" s="13" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D75" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F75" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="22" t="n">
         <v>44095</v>
       </c>
-      <c r="B75" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="C75" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D75" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="E75" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="13" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="23" t="s">
         <v>183</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="C76" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="24" t="s">
         <v>184</v>
       </c>
-      <c r="E76" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>41</v>
+      <c r="E76" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="13" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B77" s="17" t="s">
         <v>185</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>186</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>140</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="13" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>187</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>188</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>80</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="13" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>189</v>
@@ -2986,15 +2995,15 @@
         <v>190</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B80" s="17" t="s">
         <v>191</v>
@@ -3006,15 +3015,15 @@
         <v>192</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="13" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>193</v>
@@ -3026,15 +3035,15 @@
         <v>194</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="13" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B82" s="17" t="s">
         <v>195</v>
@@ -3046,35 +3055,35 @@
         <v>196</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="13" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B83" s="17" t="s">
         <v>197</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>198</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="13" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B84" s="17" t="s">
         <v>199</v>
@@ -3086,15 +3095,15 @@
         <v>200</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="13" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B85" s="17" t="s">
         <v>201</v>
@@ -3106,15 +3115,15 @@
         <v>202</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="13" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>203</v>
@@ -3126,35 +3135,35 @@
         <v>204</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="13" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B87" s="17" t="s">
         <v>205</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>206</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="13" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B88" s="17" t="s">
         <v>207</v>
@@ -3166,15 +3175,15 @@
         <v>208</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="13" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B89" s="17" t="s">
         <v>209</v>
@@ -3186,15 +3195,15 @@
         <v>210</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="13" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B90" s="17" t="s">
         <v>211</v>
@@ -3206,10 +3215,10 @@
         <v>212</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3226,15 +3235,15 @@
         <v>214</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="13" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B92" s="17" t="s">
         <v>215</v>
@@ -3246,15 +3255,15 @@
         <v>216</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="13" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B93" s="17" t="s">
         <v>217</v>
@@ -3266,10 +3275,10 @@
         <v>218</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3289,14 +3298,14 @@
         <v>23</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="13" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B95" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B95" s="17" t="s">
         <v>221</v>
       </c>
       <c r="C95" s="5" t="s">
@@ -3309,32 +3318,32 @@
         <v>23</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="13" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B97" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="13" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="C97" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D97" s="5" t="s">
+      <c r="C96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="E97" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>73</v>
+      <c r="E96" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,61 +3354,61 @@
         <v>225</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>226</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>227</v>
+        <v>75</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="13" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B99" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D99" s="5" t="s">
+      <c r="E99" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F99" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="13" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B100" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B100" s="25" t="s">
         <v>230</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>231</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="13" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>232</v>
@@ -3411,19 +3420,39 @@
         <v>233</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="103" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMH103" s="0"/>
-      <c r="AMI103" s="0"/>
-      <c r="AMJ103" s="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="13" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F102" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="104" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMH104" s="0"/>
+      <c r="AMI104" s="0"/>
+      <c r="AMJ104" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F101">
+  <autoFilter ref="A1:F102">
     <filterColumn colId="5">
       <filters>
         <filter val="Fixed?"/>
@@ -3444,98 +3473,99 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="#11"/>
-    <hyperlink ref="B5" r:id="rId2" display="#1309"/>
-    <hyperlink ref="B6" r:id="rId3" display="#1176"/>
-    <hyperlink ref="B7" r:id="rId4" display="#1171"/>
-    <hyperlink ref="B8" r:id="rId5" display="#1164"/>
-    <hyperlink ref="B9" r:id="rId6" display="#9"/>
-    <hyperlink ref="B10" r:id="rId7" display="#1163"/>
-    <hyperlink ref="B11" r:id="rId8" display="#1161"/>
-    <hyperlink ref="B12" r:id="rId9" display="#1690"/>
-    <hyperlink ref="B14" r:id="rId10" display="#1155"/>
-    <hyperlink ref="B15" r:id="rId11" display="#1150"/>
-    <hyperlink ref="B16" r:id="rId12" display="#1151"/>
-    <hyperlink ref="B17" r:id="rId13" display="#1200"/>
-    <hyperlink ref="B18" r:id="rId14" display="#1681"/>
-    <hyperlink ref="B19" r:id="rId15" display="#1142"/>
-    <hyperlink ref="B20" r:id="rId16" display="#8"/>
-    <hyperlink ref="B21" r:id="rId17" display="#1674"/>
-    <hyperlink ref="B22" r:id="rId18" display="#1672"/>
-    <hyperlink ref="B23" r:id="rId19" display="#1669"/>
-    <hyperlink ref="B24" r:id="rId20" display="#1670"/>
-    <hyperlink ref="B25" r:id="rId21" display="#1184"/>
-    <hyperlink ref="B26" r:id="rId22" display="#49"/>
-    <hyperlink ref="B27" r:id="rId23" display="#1140"/>
-    <hyperlink ref="B28" r:id="rId24" display="#1132"/>
-    <hyperlink ref="B30" r:id="rId25" display="#1125"/>
-    <hyperlink ref="B31" r:id="rId26" display="#1641"/>
-    <hyperlink ref="B32" r:id="rId27" display="#1124"/>
-    <hyperlink ref="B33" r:id="rId28" display="#1122"/>
-    <hyperlink ref="B34" r:id="rId29" display="#43"/>
-    <hyperlink ref="B35" r:id="rId30" display="#1622"/>
-    <hyperlink ref="B37" r:id="rId31" display="#38"/>
-    <hyperlink ref="B38" r:id="rId32" display="#1621"/>
-    <hyperlink ref="B39" r:id="rId33" display="#1616"/>
-    <hyperlink ref="B40" r:id="rId34" display="#37"/>
-    <hyperlink ref="B41" r:id="rId35" display="#36"/>
-    <hyperlink ref="B42" r:id="rId36" display="#1101"/>
-    <hyperlink ref="B43" r:id="rId37" display="#1099"/>
-    <hyperlink ref="B44" r:id="rId38" display="#1098"/>
-    <hyperlink ref="B45" r:id="rId39" display="#1617"/>
-    <hyperlink ref="B46" r:id="rId40" display="#1092"/>
-    <hyperlink ref="B47" r:id="rId41" display="#1128"/>
-    <hyperlink ref="B48" r:id="rId42" display="#1090"/>
-    <hyperlink ref="B49" r:id="rId43" display="#1608"/>
-    <hyperlink ref="B50" r:id="rId44" display="#35"/>
-    <hyperlink ref="B52" r:id="rId45" display="#1070"/>
-    <hyperlink ref="B53" r:id="rId46" display="#1592"/>
-    <hyperlink ref="B54" r:id="rId47" display="#1591"/>
-    <hyperlink ref="B55" r:id="rId48" display="#1578"/>
-    <hyperlink ref="B56" r:id="rId49" display="#41"/>
-    <hyperlink ref="B57" r:id="rId50" display="#42"/>
-    <hyperlink ref="B58" r:id="rId51" display="#1566"/>
-    <hyperlink ref="B59" r:id="rId52" display="#1565"/>
-    <hyperlink ref="B60" r:id="rId53" display="#1046"/>
-    <hyperlink ref="B61" r:id="rId54" display="#1559"/>
-    <hyperlink ref="B62" r:id="rId55" display="#1038"/>
-    <hyperlink ref="B63" r:id="rId56" display="#1037"/>
-    <hyperlink ref="B64" r:id="rId57" display="#1020"/>
-    <hyperlink ref="B65" r:id="rId58" display="#1032"/>
-    <hyperlink ref="B66" r:id="rId59" display="#1546"/>
-    <hyperlink ref="B67" r:id="rId60" display="#1027"/>
-    <hyperlink ref="B68" r:id="rId61" display="#1529"/>
-    <hyperlink ref="B70" r:id="rId62" display="#1527"/>
-    <hyperlink ref="B71" r:id="rId63" display="#558"/>
-    <hyperlink ref="B72" r:id="rId64" display="#1005"/>
-    <hyperlink ref="B73" r:id="rId65" display="#1020"/>
-    <hyperlink ref="B74" r:id="rId66" display="#993"/>
-    <hyperlink ref="B75" r:id="rId67" display="#1520"/>
-    <hyperlink ref="B76" r:id="rId68" display="#1519"/>
-    <hyperlink ref="B77" r:id="rId69" display="#969"/>
-    <hyperlink ref="B78" r:id="rId70" display="#1003"/>
-    <hyperlink ref="B79" r:id="rId71" display="#1015"/>
-    <hyperlink ref="B80" r:id="rId72" display="#1002"/>
-    <hyperlink ref="B81" r:id="rId73" display="#1471"/>
-    <hyperlink ref="B82" r:id="rId74" display="#1497"/>
-    <hyperlink ref="B83" r:id="rId75" display="#947"/>
-    <hyperlink ref="B84" r:id="rId76" display="#933"/>
-    <hyperlink ref="B85" r:id="rId77" display="#932"/>
-    <hyperlink ref="B86" r:id="rId78" display="#931"/>
-    <hyperlink ref="B87" r:id="rId79" display="#987"/>
-    <hyperlink ref="B88" r:id="rId80" display="#988"/>
-    <hyperlink ref="B89" r:id="rId81" display="#982"/>
-    <hyperlink ref="B90" r:id="rId82" display="#979"/>
-    <hyperlink ref="B91" r:id="rId83" display="#977"/>
-    <hyperlink ref="B92" r:id="rId84" display="#975"/>
-    <hyperlink ref="B93" r:id="rId85" display="#1445"/>
-    <hyperlink ref="B94" r:id="rId86" display="#1444"/>
-    <hyperlink ref="B95" r:id="rId87" display="#1427"/>
-    <hyperlink ref="B97" r:id="rId88" display="#23"/>
-    <hyperlink ref="B98" r:id="rId89" display="#22"/>
-    <hyperlink ref="B99" r:id="rId90" display="#18"/>
-    <hyperlink ref="B100" r:id="rId91" display="#1207"/>
-    <hyperlink ref="B101" r:id="rId92" display="#245"/>
+    <hyperlink ref="B4" r:id="rId1" display="#1185"/>
+    <hyperlink ref="B5" r:id="rId2" display="#11"/>
+    <hyperlink ref="B6" r:id="rId3" display="#1309"/>
+    <hyperlink ref="B7" r:id="rId4" display="#1176"/>
+    <hyperlink ref="B8" r:id="rId5" display="#1171"/>
+    <hyperlink ref="B9" r:id="rId6" display="#1164"/>
+    <hyperlink ref="B10" r:id="rId7" display="#9"/>
+    <hyperlink ref="B11" r:id="rId8" display="#1163"/>
+    <hyperlink ref="B12" r:id="rId9" display="#1161"/>
+    <hyperlink ref="B13" r:id="rId10" display="#1690"/>
+    <hyperlink ref="B15" r:id="rId11" display="#1155"/>
+    <hyperlink ref="B16" r:id="rId12" display="#1150"/>
+    <hyperlink ref="B17" r:id="rId13" display="#1151"/>
+    <hyperlink ref="B18" r:id="rId14" display="#1200"/>
+    <hyperlink ref="B19" r:id="rId15" display="#1681"/>
+    <hyperlink ref="B20" r:id="rId16" display="#1142"/>
+    <hyperlink ref="B21" r:id="rId17" display="#8"/>
+    <hyperlink ref="B22" r:id="rId18" display="#1674"/>
+    <hyperlink ref="B23" r:id="rId19" display="#1672"/>
+    <hyperlink ref="B24" r:id="rId20" display="#1669"/>
+    <hyperlink ref="B25" r:id="rId21" display="#1670"/>
+    <hyperlink ref="B26" r:id="rId22" display="#1184"/>
+    <hyperlink ref="B27" r:id="rId23" display="#49"/>
+    <hyperlink ref="B28" r:id="rId24" display="#1140"/>
+    <hyperlink ref="B29" r:id="rId25" display="#1132"/>
+    <hyperlink ref="B31" r:id="rId26" display="#1125"/>
+    <hyperlink ref="B32" r:id="rId27" display="#1641"/>
+    <hyperlink ref="B33" r:id="rId28" display="#1124"/>
+    <hyperlink ref="B34" r:id="rId29" display="#1122"/>
+    <hyperlink ref="B35" r:id="rId30" display="#43"/>
+    <hyperlink ref="B36" r:id="rId31" display="#1622"/>
+    <hyperlink ref="B38" r:id="rId32" display="#38"/>
+    <hyperlink ref="B39" r:id="rId33" display="#1621"/>
+    <hyperlink ref="B40" r:id="rId34" display="#1616"/>
+    <hyperlink ref="B41" r:id="rId35" display="#37"/>
+    <hyperlink ref="B42" r:id="rId36" display="#36"/>
+    <hyperlink ref="B43" r:id="rId37" display="#1101"/>
+    <hyperlink ref="B44" r:id="rId38" display="#1099"/>
+    <hyperlink ref="B45" r:id="rId39" display="#1098"/>
+    <hyperlink ref="B46" r:id="rId40" display="#1617"/>
+    <hyperlink ref="B47" r:id="rId41" display="#1092"/>
+    <hyperlink ref="B48" r:id="rId42" display="#1128"/>
+    <hyperlink ref="B49" r:id="rId43" display="#1090"/>
+    <hyperlink ref="B50" r:id="rId44" display="#1608"/>
+    <hyperlink ref="B51" r:id="rId45" display="#35"/>
+    <hyperlink ref="B53" r:id="rId46" display="#1070"/>
+    <hyperlink ref="B54" r:id="rId47" display="#1592"/>
+    <hyperlink ref="B55" r:id="rId48" display="#1591"/>
+    <hyperlink ref="B56" r:id="rId49" display="#1578"/>
+    <hyperlink ref="B57" r:id="rId50" display="#41"/>
+    <hyperlink ref="B58" r:id="rId51" display="#42"/>
+    <hyperlink ref="B59" r:id="rId52" display="#1566"/>
+    <hyperlink ref="B60" r:id="rId53" display="#1565"/>
+    <hyperlink ref="B61" r:id="rId54" display="#1046"/>
+    <hyperlink ref="B62" r:id="rId55" display="#1559"/>
+    <hyperlink ref="B63" r:id="rId56" display="#1038"/>
+    <hyperlink ref="B64" r:id="rId57" display="#1037"/>
+    <hyperlink ref="B65" r:id="rId58" display="#1020"/>
+    <hyperlink ref="B66" r:id="rId59" display="#1032"/>
+    <hyperlink ref="B67" r:id="rId60" display="#1546"/>
+    <hyperlink ref="B68" r:id="rId61" display="#1027"/>
+    <hyperlink ref="B69" r:id="rId62" display="#1529"/>
+    <hyperlink ref="B71" r:id="rId63" display="#1527"/>
+    <hyperlink ref="B72" r:id="rId64" display="#558"/>
+    <hyperlink ref="B73" r:id="rId65" display="#1005"/>
+    <hyperlink ref="B74" r:id="rId66" display="#1020"/>
+    <hyperlink ref="B75" r:id="rId67" display="#993"/>
+    <hyperlink ref="B76" r:id="rId68" display="#1520"/>
+    <hyperlink ref="B77" r:id="rId69" display="#1519"/>
+    <hyperlink ref="B78" r:id="rId70" display="#969"/>
+    <hyperlink ref="B79" r:id="rId71" display="#1003"/>
+    <hyperlink ref="B80" r:id="rId72" display="#1015"/>
+    <hyperlink ref="B81" r:id="rId73" display="#1002"/>
+    <hyperlink ref="B82" r:id="rId74" display="#1471"/>
+    <hyperlink ref="B83" r:id="rId75" display="#1497"/>
+    <hyperlink ref="B84" r:id="rId76" display="#947"/>
+    <hyperlink ref="B85" r:id="rId77" display="#933"/>
+    <hyperlink ref="B86" r:id="rId78" display="#932"/>
+    <hyperlink ref="B87" r:id="rId79" display="#931"/>
+    <hyperlink ref="B88" r:id="rId80" display="#987"/>
+    <hyperlink ref="B89" r:id="rId81" display="#988"/>
+    <hyperlink ref="B90" r:id="rId82" display="#982"/>
+    <hyperlink ref="B91" r:id="rId83" display="#979"/>
+    <hyperlink ref="B92" r:id="rId84" display="#977"/>
+    <hyperlink ref="B93" r:id="rId85" display="#975"/>
+    <hyperlink ref="B94" r:id="rId86" display="#1445"/>
+    <hyperlink ref="B95" r:id="rId87" display="#1444"/>
+    <hyperlink ref="B96" r:id="rId88" display="#1427"/>
+    <hyperlink ref="B98" r:id="rId89" display="#23"/>
+    <hyperlink ref="B99" r:id="rId90" display="#22"/>
+    <hyperlink ref="B100" r:id="rId91" display="#18"/>
+    <hyperlink ref="B101" r:id="rId92" display="#1207"/>
+    <hyperlink ref="B102" r:id="rId93" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -3544,7 +3574,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId93"/>
+  <drawing r:id="rId94"/>
 </worksheet>
 </file>
 
@@ -3577,10 +3607,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -3589,10 +3619,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added OmegT issue #1708
</commit_message>
<xml_diff>
--- a/tickets/OmegaT_issues_nopw.xlsx
+++ b/tickets/OmegaT_issues_nopw.xlsx
@@ -13,7 +13,7 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$102</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$103</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Sheet_Title" vbProcedure="false">"Devs"</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">#REF!</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="242">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -123,6 +123,18 @@
     <t xml:space="preserve">WIP</t>
   </si>
   <si>
+    <t xml:space="preserve">#1708</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improve colors in the list of project files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
     <t xml:space="preserve">#1185</t>
   </si>
   <si>
@@ -162,9 +174,6 @@
     <t xml:space="preserve">Enforced translations lose background color</t>
   </si>
   <si>
-    <t xml:space="preserve">Open</t>
-  </si>
-  <si>
     <t xml:space="preserve">#1164</t>
   </si>
   <si>
@@ -178,9 +187,6 @@
   </si>
   <si>
     <t xml:space="preserve">Add property in config to remove mappings (to pack as offline project)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RFE</t>
   </si>
   <si>
     <t xml:space="preserve">#1163</t>
@@ -1381,14 +1387,14 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ104"/>
+  <dimension ref="A1:AMJ105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1444,7 +1450,7 @@
     </row>
     <row r="4" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
-        <v>45104</v>
+        <v>45110</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>30</v>
@@ -1456,10 +1462,10 @@
         <v>31</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
@@ -1467,13 +1473,13 @@
     </row>
     <row r="5" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="n">
-        <v>45094</v>
+        <v>45104</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>35</v>
@@ -1490,22 +1496,22 @@
     </row>
     <row r="6" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
-        <v>45069</v>
+        <v>45094</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
@@ -1516,13 +1522,13 @@
         <v>45069</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>9</v>
@@ -1536,22 +1542,22 @@
     </row>
     <row r="8" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
-        <v>45064</v>
+        <v>45069</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AMH8" s="0"/>
       <c r="AMI8" s="0"/>
@@ -1559,22 +1565,22 @@
     </row>
     <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
-        <v>45049</v>
+        <v>45064</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="AMH9" s="0"/>
       <c r="AMI9" s="0"/>
@@ -1587,17 +1593,17 @@
       <c r="B10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>34</v>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
@@ -1605,22 +1611,22 @@
     </row>
     <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="n">
-        <v>45044</v>
+        <v>45049</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>7</v>
+      <c r="C11" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>51</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="AMH11" s="0"/>
       <c r="AMI11" s="0"/>
@@ -1628,7 +1634,7 @@
     </row>
     <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
-        <v>45040</v>
+        <v>45044</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>52</v>
@@ -1643,7 +1649,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AMH12" s="0"/>
       <c r="AMI12" s="0"/>
@@ -1651,7 +1657,7 @@
     </row>
     <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>54</v>
@@ -1663,10 +1669,10 @@
         <v>55</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AMH13" s="0"/>
       <c r="AMI13" s="0"/>
@@ -1674,16 +1680,22 @@
     </row>
     <row r="14" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>57</v>
       </c>
+      <c r="E14" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="F14" s="9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
@@ -1691,22 +1703,16 @@
     </row>
     <row r="15" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B15" s="11" t="s">
+        <v>44996</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="F15" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="AMH15" s="0"/>
       <c r="AMI15" s="0"/>
@@ -1714,7 +1720,7 @@
     </row>
     <row r="16" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>60</v>
@@ -1729,7 +1735,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
@@ -1752,7 +1758,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AMH17" s="0"/>
       <c r="AMI17" s="0"/>
@@ -1760,13 +1766,13 @@
     </row>
     <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>65</v>
@@ -1775,7 +1781,7 @@
         <v>9</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="AMH18" s="0"/>
       <c r="AMI18" s="0"/>
@@ -1783,22 +1789,22 @@
     </row>
     <row r="19" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="AMH19" s="0"/>
       <c r="AMI19" s="0"/>
@@ -1806,7 +1812,7 @@
     </row>
     <row r="20" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="n">
-        <v>44972</v>
+        <v>44981</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>69</v>
@@ -1818,33 +1824,33 @@
         <v>70</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="AMH20" s="0"/>
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B21" s="14" t="s">
+    <row r="21" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>43</v>
+      <c r="E21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="AMH21" s="0"/>
       <c r="AMI21" s="0"/>
@@ -1852,22 +1858,22 @@
     </row>
     <row r="22" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>74</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="AMH22" s="0"/>
       <c r="AMI22" s="0"/>
@@ -1875,22 +1881,22 @@
     </row>
     <row r="23" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="12" t="s">
+      <c r="E23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="AMH23" s="0"/>
       <c r="AMI23" s="0"/>
@@ -1898,7 +1904,7 @@
     </row>
     <row r="24" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>78</v>
@@ -1910,10 +1916,10 @@
         <v>79</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AMH24" s="0"/>
       <c r="AMI24" s="0"/>
@@ -1933,10 +1939,10 @@
         <v>81</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="AMH25" s="0"/>
       <c r="AMI25" s="0"/>
@@ -1944,22 +1950,22 @@
     </row>
     <row r="26" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="n">
-        <v>44949</v>
+        <v>44952</v>
       </c>
       <c r="B26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="12" t="s">
+      <c r="E26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
@@ -1967,22 +1973,22 @@
     </row>
     <row r="27" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="n">
-        <v>44948</v>
+        <v>44949</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>85</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>86</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="AMH27" s="0"/>
       <c r="AMI27" s="0"/>
@@ -1990,125 +1996,125 @@
     </row>
     <row r="28" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>88</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
       <c r="AMJ28" s="0"/>
     </row>
-    <row r="29" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B29" s="16" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>91</v>
-      </c>
       <c r="E29" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
       <c r="AMJ29" s="0"/>
     </row>
-    <row r="30" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
+    <row r="30" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>29</v>
+      <c r="C30" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="AMH30" s="0"/>
       <c r="AMI30" s="0"/>
       <c r="AMJ30" s="0"/>
     </row>
-    <row r="31" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="5" t="s">
+    <row r="31" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>43</v>
+      <c r="F31" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMH31" s="0"/>
       <c r="AMI31" s="0"/>
       <c r="AMJ31" s="0"/>
     </row>
-    <row r="32" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B32" s="14" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="12" t="s">
+      <c r="C32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>43</v>
+      <c r="E32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="AMH32" s="0"/>
       <c r="AMI32" s="0"/>
       <c r="AMJ32" s="0"/>
     </row>
-    <row r="33" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" s="12" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B33" s="17" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="C33" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="E33" s="12" t="s">
         <v>32</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>33</v>
       </c>
       <c r="AMH33" s="0"/>
       <c r="AMI33" s="0"/>
@@ -2116,7 +2122,7 @@
     </row>
     <row r="34" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>99</v>
@@ -2128,112 +2134,115 @@
         <v>100</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="AMH34" s="0"/>
       <c r="AMI34" s="0"/>
       <c r="AMJ34" s="0"/>
     </row>
-    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B35" s="18" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="E35" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>82</v>
-      </c>
+      <c r="AMH35" s="0"/>
+      <c r="AMI35" s="0"/>
+      <c r="AMJ35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B36" s="17" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>106</v>
       </c>
       <c r="E36" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13" t="n">
+        <v>373466</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="n">
-        <v>44743</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="F37" s="5" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>108</v>
+        <v>44743</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="F38" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B39" s="20" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B39" s="19" t="s">
         <v>110</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>111</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>112</v>
@@ -2245,90 +2254,90 @@
         <v>113</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B41" s="21" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B41" s="20" t="s">
         <v>114</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13" t="n">
-        <v>44659</v>
+        <v>44695</v>
       </c>
       <c r="B42" s="21" t="s">
         <v>116</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>117</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="13" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B43" s="20" t="s">
+        <v>44659</v>
+      </c>
+      <c r="B43" s="21" t="s">
         <v>118</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>119</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B44" s="17" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C44" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,15 +2354,15 @@
         <v>124</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>125</v>
@@ -2365,15 +2374,15 @@
         <v>126</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>127</v>
@@ -2385,57 +2394,57 @@
         <v>128</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B48" s="17" t="s">
         <v>129</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>130</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="13" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>131</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>132</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="13" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B50" s="20" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B50" s="17" t="s">
         <v>133</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2445,60 +2454,60 @@
         <v>134</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="13" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B51" s="17" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B51" s="20" t="s">
         <v>135</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>136</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="13" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B52" s="17" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="13" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B53" s="17" t="s">
+      <c r="C52" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="5" t="s">
+      <c r="E52" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="13" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>140</v>
@@ -2510,10 +2519,10 @@
         <v>141</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,24 +2530,24 @@
         <v>44460</v>
       </c>
       <c r="B55" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="13" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B56" s="17" t="s">
         <v>145</v>
@@ -2553,72 +2562,72 @@
         <v>23</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="13" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>147</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>148</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>101</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="13" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B58" s="21" t="s">
+        <v>44326</v>
+      </c>
+      <c r="B58" s="17" t="s">
         <v>149</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>150</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="13" t="n">
         <v>44325</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="21" t="s">
         <v>151</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B60" s="17" t="s">
         <v>153</v>
@@ -2630,15 +2639,15 @@
         <v>154</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="13" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>155</v>
@@ -2650,37 +2659,37 @@
         <v>156</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>157</v>
+        <v>36</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="13" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B62" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="5" t="s">
+      <c r="E62" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="13" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B63" s="17" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>160</v>
       </c>
       <c r="C63" s="5" t="s">
@@ -2690,15 +2699,15 @@
         <v>161</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="13" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B64" s="17" t="s">
         <v>162</v>
@@ -2710,57 +2719,57 @@
         <v>163</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="22" t="n">
+      <c r="A65" s="13" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="22" t="n">
         <v>44231</v>
       </c>
-      <c r="B65" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C65" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E65" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="13" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" s="5" t="s">
+      <c r="C66" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="E66" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F66" s="24" t="s">
         <v>167</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="13" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B67" s="20" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B67" s="17" t="s">
         <v>168</v>
       </c>
       <c r="C67" s="5" t="s">
@@ -2770,17 +2779,17 @@
         <v>169</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="13" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B68" s="17" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B68" s="20" t="s">
         <v>170</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -2790,10 +2799,10 @@
         <v>171</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2810,40 +2819,40 @@
         <v>173</v>
       </c>
       <c r="E69" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="13" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F69" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="13" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>43</v>
+      <c r="F70" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="13" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B72" s="17" t="s">
         <v>176</v>
@@ -2852,158 +2861,158 @@
         <v>7</v>
       </c>
       <c r="D72" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="13" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="22" t="n">
+      <c r="E73" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="22" t="n">
         <v>44146</v>
       </c>
-      <c r="B73" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="C73" s="24" t="s">
+      <c r="B74" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D73" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="E73" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="13" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="E74" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>43</v>
+      <c r="E74" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="13" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>182</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="22" t="n">
+      <c r="A76" s="13" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="22" t="n">
         <v>44095</v>
       </c>
-      <c r="B76" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="C76" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="E76" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F76" s="24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="13" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="C77" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="5" t="s">
+      <c r="C77" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="E77" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>43</v>
+      <c r="E77" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="13" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>187</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>188</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>142</v>
+        <v>33</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="13" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B79" s="17" t="s">
         <v>189</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>190</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>82</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="13" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B80" s="17" t="s">
         <v>191</v>
@@ -3015,15 +3024,15 @@
         <v>192</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="13" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>193</v>
@@ -3035,15 +3044,15 @@
         <v>194</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="13" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B82" s="17" t="s">
         <v>195</v>
@@ -3055,15 +3064,15 @@
         <v>196</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="13" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B83" s="17" t="s">
         <v>197</v>
@@ -3075,35 +3084,35 @@
         <v>198</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="13" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B84" s="17" t="s">
         <v>199</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>200</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="13" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B85" s="17" t="s">
         <v>201</v>
@@ -3115,15 +3124,15 @@
         <v>202</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="13" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>203</v>
@@ -3135,15 +3144,15 @@
         <v>204</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="13" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B87" s="17" t="s">
         <v>205</v>
@@ -3155,35 +3164,35 @@
         <v>206</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="13" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B88" s="17" t="s">
         <v>207</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>208</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="13" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B89" s="17" t="s">
         <v>209</v>
@@ -3195,15 +3204,15 @@
         <v>210</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="13" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B90" s="17" t="s">
         <v>211</v>
@@ -3215,15 +3224,15 @@
         <v>212</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="13" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B91" s="17" t="s">
         <v>213</v>
@@ -3235,10 +3244,10 @@
         <v>214</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3255,15 +3264,15 @@
         <v>216</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="13" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B93" s="17" t="s">
         <v>217</v>
@@ -3275,15 +3284,15 @@
         <v>218</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="13" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B94" s="17" t="s">
         <v>219</v>
@@ -3295,10 +3304,10 @@
         <v>220</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3318,14 +3327,14 @@
         <v>23</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="13" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B96" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B96" s="17" t="s">
         <v>223</v>
       </c>
       <c r="C96" s="5" t="s">
@@ -3338,32 +3347,32 @@
         <v>23</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="13" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B98" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="13" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B97" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C98" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D98" s="5" t="s">
+      <c r="C97" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="E98" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>75</v>
+      <c r="E97" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3374,61 +3383,61 @@
         <v>227</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>228</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>229</v>
+        <v>77</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="13" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B100" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D100" s="5" t="s">
+      <c r="E100" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F100" s="5" t="s">
         <v>231</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="13" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B101" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B101" s="25" t="s">
         <v>232</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>233</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>234</v>
@@ -3440,19 +3449,39 @@
         <v>235</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="104" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMH104" s="0"/>
-      <c r="AMI104" s="0"/>
-      <c r="AMJ104" s="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="13" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="105" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMH105" s="0"/>
+      <c r="AMI105" s="0"/>
+      <c r="AMJ105" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F102">
+  <autoFilter ref="A1:F103">
     <filterColumn colId="5">
       <filters>
         <filter val="Fixed?"/>
@@ -3473,99 +3502,100 @@
     </filterColumn>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="#1185"/>
-    <hyperlink ref="B5" r:id="rId2" display="#11"/>
-    <hyperlink ref="B6" r:id="rId3" display="#1309"/>
-    <hyperlink ref="B7" r:id="rId4" display="#1176"/>
-    <hyperlink ref="B8" r:id="rId5" display="#1171"/>
-    <hyperlink ref="B9" r:id="rId6" display="#1164"/>
-    <hyperlink ref="B10" r:id="rId7" display="#9"/>
-    <hyperlink ref="B11" r:id="rId8" display="#1163"/>
-    <hyperlink ref="B12" r:id="rId9" display="#1161"/>
-    <hyperlink ref="B13" r:id="rId10" display="#1690"/>
-    <hyperlink ref="B15" r:id="rId11" display="#1155"/>
-    <hyperlink ref="B16" r:id="rId12" display="#1150"/>
-    <hyperlink ref="B17" r:id="rId13" display="#1151"/>
-    <hyperlink ref="B18" r:id="rId14" display="#1200"/>
-    <hyperlink ref="B19" r:id="rId15" display="#1681"/>
-    <hyperlink ref="B20" r:id="rId16" display="#1142"/>
-    <hyperlink ref="B21" r:id="rId17" display="#8"/>
-    <hyperlink ref="B22" r:id="rId18" display="#1674"/>
-    <hyperlink ref="B23" r:id="rId19" display="#1672"/>
-    <hyperlink ref="B24" r:id="rId20" display="#1669"/>
-    <hyperlink ref="B25" r:id="rId21" display="#1670"/>
-    <hyperlink ref="B26" r:id="rId22" display="#1184"/>
-    <hyperlink ref="B27" r:id="rId23" display="#49"/>
-    <hyperlink ref="B28" r:id="rId24" display="#1140"/>
-    <hyperlink ref="B29" r:id="rId25" display="#1132"/>
-    <hyperlink ref="B31" r:id="rId26" display="#1125"/>
-    <hyperlink ref="B32" r:id="rId27" display="#1641"/>
-    <hyperlink ref="B33" r:id="rId28" display="#1124"/>
-    <hyperlink ref="B34" r:id="rId29" display="#1122"/>
-    <hyperlink ref="B35" r:id="rId30" display="#43"/>
-    <hyperlink ref="B36" r:id="rId31" display="#1622"/>
-    <hyperlink ref="B38" r:id="rId32" display="#38"/>
-    <hyperlink ref="B39" r:id="rId33" display="#1621"/>
-    <hyperlink ref="B40" r:id="rId34" display="#1616"/>
-    <hyperlink ref="B41" r:id="rId35" display="#37"/>
-    <hyperlink ref="B42" r:id="rId36" display="#36"/>
-    <hyperlink ref="B43" r:id="rId37" display="#1101"/>
-    <hyperlink ref="B44" r:id="rId38" display="#1099"/>
-    <hyperlink ref="B45" r:id="rId39" display="#1098"/>
-    <hyperlink ref="B46" r:id="rId40" display="#1617"/>
-    <hyperlink ref="B47" r:id="rId41" display="#1092"/>
-    <hyperlink ref="B48" r:id="rId42" display="#1128"/>
-    <hyperlink ref="B49" r:id="rId43" display="#1090"/>
-    <hyperlink ref="B50" r:id="rId44" display="#1608"/>
-    <hyperlink ref="B51" r:id="rId45" display="#35"/>
-    <hyperlink ref="B53" r:id="rId46" display="#1070"/>
-    <hyperlink ref="B54" r:id="rId47" display="#1592"/>
-    <hyperlink ref="B55" r:id="rId48" display="#1591"/>
-    <hyperlink ref="B56" r:id="rId49" display="#1578"/>
-    <hyperlink ref="B57" r:id="rId50" display="#41"/>
-    <hyperlink ref="B58" r:id="rId51" display="#42"/>
-    <hyperlink ref="B59" r:id="rId52" display="#1566"/>
-    <hyperlink ref="B60" r:id="rId53" display="#1565"/>
-    <hyperlink ref="B61" r:id="rId54" display="#1046"/>
-    <hyperlink ref="B62" r:id="rId55" display="#1559"/>
-    <hyperlink ref="B63" r:id="rId56" display="#1038"/>
-    <hyperlink ref="B64" r:id="rId57" display="#1037"/>
-    <hyperlink ref="B65" r:id="rId58" display="#1020"/>
-    <hyperlink ref="B66" r:id="rId59" display="#1032"/>
-    <hyperlink ref="B67" r:id="rId60" display="#1546"/>
-    <hyperlink ref="B68" r:id="rId61" display="#1027"/>
-    <hyperlink ref="B69" r:id="rId62" display="#1529"/>
-    <hyperlink ref="B71" r:id="rId63" display="#1527"/>
-    <hyperlink ref="B72" r:id="rId64" display="#558"/>
-    <hyperlink ref="B73" r:id="rId65" display="#1005"/>
-    <hyperlink ref="B74" r:id="rId66" display="#1020"/>
-    <hyperlink ref="B75" r:id="rId67" display="#993"/>
-    <hyperlink ref="B76" r:id="rId68" display="#1520"/>
-    <hyperlink ref="B77" r:id="rId69" display="#1519"/>
-    <hyperlink ref="B78" r:id="rId70" display="#969"/>
-    <hyperlink ref="B79" r:id="rId71" display="#1003"/>
-    <hyperlink ref="B80" r:id="rId72" display="#1015"/>
-    <hyperlink ref="B81" r:id="rId73" display="#1002"/>
-    <hyperlink ref="B82" r:id="rId74" display="#1471"/>
-    <hyperlink ref="B83" r:id="rId75" display="#1497"/>
-    <hyperlink ref="B84" r:id="rId76" display="#947"/>
-    <hyperlink ref="B85" r:id="rId77" display="#933"/>
-    <hyperlink ref="B86" r:id="rId78" display="#932"/>
-    <hyperlink ref="B87" r:id="rId79" display="#931"/>
-    <hyperlink ref="B88" r:id="rId80" display="#987"/>
-    <hyperlink ref="B89" r:id="rId81" display="#988"/>
-    <hyperlink ref="B90" r:id="rId82" display="#982"/>
-    <hyperlink ref="B91" r:id="rId83" display="#979"/>
-    <hyperlink ref="B92" r:id="rId84" display="#977"/>
-    <hyperlink ref="B93" r:id="rId85" display="#975"/>
-    <hyperlink ref="B94" r:id="rId86" display="#1445"/>
-    <hyperlink ref="B95" r:id="rId87" display="#1444"/>
-    <hyperlink ref="B96" r:id="rId88" display="#1427"/>
-    <hyperlink ref="B98" r:id="rId89" display="#23"/>
-    <hyperlink ref="B99" r:id="rId90" display="#22"/>
-    <hyperlink ref="B100" r:id="rId91" display="#18"/>
-    <hyperlink ref="B101" r:id="rId92" display="#1207"/>
-    <hyperlink ref="B102" r:id="rId93" display="#245"/>
+    <hyperlink ref="B4" r:id="rId1" display="#1708"/>
+    <hyperlink ref="B5" r:id="rId2" display="#1185"/>
+    <hyperlink ref="B6" r:id="rId3" display="#11"/>
+    <hyperlink ref="B7" r:id="rId4" display="#1309"/>
+    <hyperlink ref="B8" r:id="rId5" display="#1176"/>
+    <hyperlink ref="B9" r:id="rId6" display="#1171"/>
+    <hyperlink ref="B10" r:id="rId7" display="#1164"/>
+    <hyperlink ref="B11" r:id="rId8" display="#9"/>
+    <hyperlink ref="B12" r:id="rId9" display="#1163"/>
+    <hyperlink ref="B13" r:id="rId10" display="#1161"/>
+    <hyperlink ref="B14" r:id="rId11" display="#1690"/>
+    <hyperlink ref="B16" r:id="rId12" display="#1155"/>
+    <hyperlink ref="B17" r:id="rId13" display="#1150"/>
+    <hyperlink ref="B18" r:id="rId14" display="#1151"/>
+    <hyperlink ref="B19" r:id="rId15" display="#1200"/>
+    <hyperlink ref="B20" r:id="rId16" display="#1681"/>
+    <hyperlink ref="B21" r:id="rId17" display="#1142"/>
+    <hyperlink ref="B22" r:id="rId18" display="#8"/>
+    <hyperlink ref="B23" r:id="rId19" display="#1674"/>
+    <hyperlink ref="B24" r:id="rId20" display="#1672"/>
+    <hyperlink ref="B25" r:id="rId21" display="#1669"/>
+    <hyperlink ref="B26" r:id="rId22" display="#1670"/>
+    <hyperlink ref="B27" r:id="rId23" display="#1184"/>
+    <hyperlink ref="B28" r:id="rId24" display="#49"/>
+    <hyperlink ref="B29" r:id="rId25" display="#1140"/>
+    <hyperlink ref="B30" r:id="rId26" display="#1132"/>
+    <hyperlink ref="B32" r:id="rId27" display="#1125"/>
+    <hyperlink ref="B33" r:id="rId28" display="#1641"/>
+    <hyperlink ref="B34" r:id="rId29" display="#1124"/>
+    <hyperlink ref="B35" r:id="rId30" display="#1122"/>
+    <hyperlink ref="B36" r:id="rId31" display="#43"/>
+    <hyperlink ref="B37" r:id="rId32" display="#1622"/>
+    <hyperlink ref="B39" r:id="rId33" display="#38"/>
+    <hyperlink ref="B40" r:id="rId34" display="#1621"/>
+    <hyperlink ref="B41" r:id="rId35" display="#1616"/>
+    <hyperlink ref="B42" r:id="rId36" display="#37"/>
+    <hyperlink ref="B43" r:id="rId37" display="#36"/>
+    <hyperlink ref="B44" r:id="rId38" display="#1101"/>
+    <hyperlink ref="B45" r:id="rId39" display="#1099"/>
+    <hyperlink ref="B46" r:id="rId40" display="#1098"/>
+    <hyperlink ref="B47" r:id="rId41" display="#1617"/>
+    <hyperlink ref="B48" r:id="rId42" display="#1092"/>
+    <hyperlink ref="B49" r:id="rId43" display="#1128"/>
+    <hyperlink ref="B50" r:id="rId44" display="#1090"/>
+    <hyperlink ref="B51" r:id="rId45" display="#1608"/>
+    <hyperlink ref="B52" r:id="rId46" display="#35"/>
+    <hyperlink ref="B54" r:id="rId47" display="#1070"/>
+    <hyperlink ref="B55" r:id="rId48" display="#1592"/>
+    <hyperlink ref="B56" r:id="rId49" display="#1591"/>
+    <hyperlink ref="B57" r:id="rId50" display="#1578"/>
+    <hyperlink ref="B58" r:id="rId51" display="#41"/>
+    <hyperlink ref="B59" r:id="rId52" display="#42"/>
+    <hyperlink ref="B60" r:id="rId53" display="#1566"/>
+    <hyperlink ref="B61" r:id="rId54" display="#1565"/>
+    <hyperlink ref="B62" r:id="rId55" display="#1046"/>
+    <hyperlink ref="B63" r:id="rId56" display="#1559"/>
+    <hyperlink ref="B64" r:id="rId57" display="#1038"/>
+    <hyperlink ref="B65" r:id="rId58" display="#1037"/>
+    <hyperlink ref="B66" r:id="rId59" display="#1020"/>
+    <hyperlink ref="B67" r:id="rId60" display="#1032"/>
+    <hyperlink ref="B68" r:id="rId61" display="#1546"/>
+    <hyperlink ref="B69" r:id="rId62" display="#1027"/>
+    <hyperlink ref="B70" r:id="rId63" display="#1529"/>
+    <hyperlink ref="B72" r:id="rId64" display="#1527"/>
+    <hyperlink ref="B73" r:id="rId65" display="#558"/>
+    <hyperlink ref="B74" r:id="rId66" display="#1005"/>
+    <hyperlink ref="B75" r:id="rId67" display="#1020"/>
+    <hyperlink ref="B76" r:id="rId68" display="#993"/>
+    <hyperlink ref="B77" r:id="rId69" display="#1520"/>
+    <hyperlink ref="B78" r:id="rId70" display="#1519"/>
+    <hyperlink ref="B79" r:id="rId71" display="#969"/>
+    <hyperlink ref="B80" r:id="rId72" display="#1003"/>
+    <hyperlink ref="B81" r:id="rId73" display="#1015"/>
+    <hyperlink ref="B82" r:id="rId74" display="#1002"/>
+    <hyperlink ref="B83" r:id="rId75" display="#1471"/>
+    <hyperlink ref="B84" r:id="rId76" display="#1497"/>
+    <hyperlink ref="B85" r:id="rId77" display="#947"/>
+    <hyperlink ref="B86" r:id="rId78" display="#933"/>
+    <hyperlink ref="B87" r:id="rId79" display="#932"/>
+    <hyperlink ref="B88" r:id="rId80" display="#931"/>
+    <hyperlink ref="B89" r:id="rId81" display="#987"/>
+    <hyperlink ref="B90" r:id="rId82" display="#988"/>
+    <hyperlink ref="B91" r:id="rId83" display="#982"/>
+    <hyperlink ref="B92" r:id="rId84" display="#979"/>
+    <hyperlink ref="B93" r:id="rId85" display="#977"/>
+    <hyperlink ref="B94" r:id="rId86" display="#975"/>
+    <hyperlink ref="B95" r:id="rId87" display="#1445"/>
+    <hyperlink ref="B96" r:id="rId88" display="#1444"/>
+    <hyperlink ref="B97" r:id="rId89" display="#1427"/>
+    <hyperlink ref="B99" r:id="rId90" display="#23"/>
+    <hyperlink ref="B100" r:id="rId91" display="#22"/>
+    <hyperlink ref="B101" r:id="rId92" display="#18"/>
+    <hyperlink ref="B102" r:id="rId93" display="#1207"/>
+    <hyperlink ref="B103" r:id="rId94" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -3574,7 +3604,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId94"/>
+  <drawing r:id="rId95"/>
 </worksheet>
 </file>
 
@@ -3607,10 +3637,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -3619,10 +3649,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor updates: harmonize status
</commit_message>
<xml_diff>
--- a/tickets/OmegaT_issues_nopw.xlsx
+++ b/tickets/OmegaT_issues_nopw.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="241">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -153,7 +153,7 @@
     <t xml:space="preserve">NoClassDefFoundError when packing project in OmegaT 6.1.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Solved</t>
+    <t xml:space="preserve">Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">#1309</t>
@@ -283,9 +283,6 @@
   </si>
   <si>
     <t xml:space="preserve">Reuse credentials in team projects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolved</t>
   </si>
   <si>
     <t xml:space="preserve">#1184</t>
@@ -1394,7 +1391,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1695,7 +1692,7 @@
         <v>32</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="AMH14" s="0"/>
       <c r="AMI14" s="0"/>
@@ -1965,7 +1962,7 @@
         <v>32</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="AMH26" s="0"/>
       <c r="AMI26" s="0"/>
@@ -1976,13 +1973,13 @@
         <v>44949</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>9</v>
@@ -1999,19 +1996,19 @@
         <v>44948</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>32</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="AMH28" s="0"/>
       <c r="AMI28" s="0"/>
@@ -2022,19 +2019,19 @@
         <v>44946</v>
       </c>
       <c r="B29" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>90</v>
-      </c>
       <c r="E29" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="AMH29" s="0"/>
       <c r="AMI29" s="0"/>
@@ -2045,16 +2042,16 @@
         <v>44929</v>
       </c>
       <c r="B30" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>93</v>
-      </c>
       <c r="E30" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>77</v>
@@ -2065,7 +2062,7 @@
     </row>
     <row r="31" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>29</v>
@@ -2079,16 +2076,16 @@
         <v>44879</v>
       </c>
       <c r="B32" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="E32" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>33</v>
@@ -2102,13 +2099,13 @@
         <v>44858</v>
       </c>
       <c r="B33" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="12" t="s">
         <v>97</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>98</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>32</v>
@@ -2125,16 +2122,16 @@
         <v>44855</v>
       </c>
       <c r="B34" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="E34" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F34" s="5" t="s">
         <v>36</v>
@@ -2148,19 +2145,19 @@
         <v>44844</v>
       </c>
       <c r="B35" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C35" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="AMH35" s="0"/>
       <c r="AMI35" s="0"/>
@@ -2171,19 +2168,19 @@
         <v>44757</v>
       </c>
       <c r="B36" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="E36" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,13 +2188,13 @@
         <v>373466</v>
       </c>
       <c r="B37" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>23</v>
@@ -2214,10 +2211,10 @@
         <v>7</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,16 +2222,16 @@
         <v>44740</v>
       </c>
       <c r="B39" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="E39" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>77</v>
@@ -2245,13 +2242,13 @@
         <v>44739</v>
       </c>
       <c r="B40" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>23</v>
@@ -2265,13 +2262,13 @@
         <v>44693</v>
       </c>
       <c r="B41" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>32</v>
@@ -2285,19 +2282,19 @@
         <v>44695</v>
       </c>
       <c r="B42" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>117</v>
-      </c>
       <c r="E42" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,16 +2302,16 @@
         <v>44659</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>77</v>
@@ -2325,19 +2322,19 @@
         <v>44712</v>
       </c>
       <c r="B44" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,19 +2342,19 @@
         <v>44705</v>
       </c>
       <c r="B45" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C45" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="E45" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,19 +2362,19 @@
         <v>44705</v>
       </c>
       <c r="B46" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="E46" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2385,13 +2382,13 @@
         <v>44693</v>
       </c>
       <c r="B47" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>32</v>
@@ -2405,19 +2402,19 @@
         <v>44622</v>
       </c>
       <c r="B48" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>130</v>
-      </c>
       <c r="E48" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,16 +2422,16 @@
         <v>44614</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>77</v>
@@ -2445,16 +2442,16 @@
         <v>44613</v>
       </c>
       <c r="B50" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="E50" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F50" s="5" t="s">
         <v>33</v>
@@ -2465,19 +2462,19 @@
         <v>44608</v>
       </c>
       <c r="B51" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>136</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,24 +2482,24 @@
         <v>44580</v>
       </c>
       <c r="B52" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,16 +2507,16 @@
         <v>44463</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>141</v>
-      </c>
       <c r="E54" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>33</v>
@@ -2530,19 +2527,19 @@
         <v>44460</v>
       </c>
       <c r="B55" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2550,13 +2547,13 @@
         <v>44460</v>
       </c>
       <c r="B56" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>23</v>
@@ -2570,13 +2567,13 @@
         <v>44372</v>
       </c>
       <c r="B57" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>23</v>
@@ -2590,19 +2587,19 @@
         <v>44326</v>
       </c>
       <c r="B58" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D58" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>150</v>
-      </c>
       <c r="E58" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,16 +2607,16 @@
         <v>44325</v>
       </c>
       <c r="B59" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D59" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>152</v>
-      </c>
       <c r="E59" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>77</v>
@@ -2630,13 +2627,13 @@
         <v>44325</v>
       </c>
       <c r="B60" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>23</v>
@@ -2650,13 +2647,13 @@
         <v>44321</v>
       </c>
       <c r="B61" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>32</v>
@@ -2670,19 +2667,19 @@
         <v>44316</v>
       </c>
       <c r="B62" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D62" s="5" t="s">
+      <c r="E62" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2690,13 +2687,13 @@
         <v>44279</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>161</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>23</v>
@@ -2710,16 +2707,16 @@
         <v>44257</v>
       </c>
       <c r="B64" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C64" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>163</v>
-      </c>
       <c r="E64" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>33</v>
@@ -2730,16 +2727,16 @@
         <v>44243</v>
       </c>
       <c r="B65" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="E65" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F65" s="5" t="s">
         <v>33</v>
@@ -2750,19 +2747,19 @@
         <v>44231</v>
       </c>
       <c r="B66" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C66" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E66" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F66" s="24" t="s">
         <v>166</v>
-      </c>
-      <c r="C66" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="E66" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F66" s="24" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,16 +2767,16 @@
         <v>44218</v>
       </c>
       <c r="B67" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="E67" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F67" s="5" t="s">
         <v>33</v>
@@ -2790,13 +2787,13 @@
         <v>44216</v>
       </c>
       <c r="B68" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="E68" s="5" t="s">
         <v>23</v>
@@ -2810,16 +2807,16 @@
         <v>44175</v>
       </c>
       <c r="B69" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="C69" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="E69" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F69" s="5" t="s">
         <v>33</v>
@@ -2830,13 +2827,13 @@
         <v>44175</v>
       </c>
       <c r="B70" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>175</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>23</v>
@@ -2847,7 +2844,7 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,13 +2852,13 @@
         <v>44162</v>
       </c>
       <c r="B72" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D72" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>32</v>
@@ -2875,7 +2872,7 @@
         <v>44148</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>7</v>
@@ -2884,7 +2881,7 @@
         <v>8</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F73" s="5" t="s">
         <v>33</v>
@@ -2895,19 +2892,19 @@
         <v>44146</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C74" s="24" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="E74" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F74" s="24" t="s">
         <v>180</v>
-      </c>
-      <c r="E74" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="F74" s="24" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2915,16 +2912,16 @@
         <v>44132</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F75" s="5" t="s">
         <v>33</v>
@@ -2935,16 +2932,16 @@
         <v>44103</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F76" s="5" t="s">
         <v>33</v>
@@ -2955,19 +2952,19 @@
         <v>44095</v>
       </c>
       <c r="B77" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C77" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="24" t="s">
         <v>185</v>
-      </c>
-      <c r="C77" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D77" s="24" t="s">
-        <v>186</v>
       </c>
       <c r="E77" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2975,13 +2972,13 @@
         <v>44095</v>
       </c>
       <c r="B78" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>32</v>
@@ -2995,19 +2992,19 @@
         <v>44057</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3015,19 +3012,19 @@
         <v>44028</v>
       </c>
       <c r="B80" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C80" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="E80" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3035,16 +3032,16 @@
         <v>44064</v>
       </c>
       <c r="B81" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C81" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>194</v>
-      </c>
       <c r="E81" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>33</v>
@@ -3055,19 +3052,19 @@
         <v>44028</v>
       </c>
       <c r="B82" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C82" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D82" s="5" t="s">
-        <v>196</v>
-      </c>
       <c r="E82" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3075,13 +3072,13 @@
         <v>44016</v>
       </c>
       <c r="B83" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D83" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>32</v>
@@ -3095,13 +3092,13 @@
         <v>44010</v>
       </c>
       <c r="B84" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>23</v>
@@ -3115,13 +3112,13 @@
         <v>43995</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>32</v>
@@ -3135,19 +3132,19 @@
         <v>43948</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3155,16 +3152,16 @@
         <v>43947</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F87" s="5" t="s">
         <v>77</v>
@@ -3175,13 +3172,13 @@
         <v>43936</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E88" s="5" t="s">
         <v>32</v>
@@ -3195,16 +3192,16 @@
         <v>43929</v>
       </c>
       <c r="B89" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C89" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="E89" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>33</v>
@@ -3215,19 +3212,19 @@
         <v>43891</v>
       </c>
       <c r="B90" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C90" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="E90" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3235,16 +3232,16 @@
         <v>43885</v>
       </c>
       <c r="B91" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C91" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" s="5" t="s">
-        <v>214</v>
-      </c>
       <c r="E91" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F91" s="5" t="s">
         <v>33</v>
@@ -3255,16 +3252,16 @@
         <v>43857</v>
       </c>
       <c r="B92" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C92" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>216</v>
-      </c>
       <c r="E92" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F92" s="5" t="s">
         <v>33</v>
@@ -3275,16 +3272,16 @@
         <v>43857</v>
       </c>
       <c r="B93" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C93" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D93" s="5" t="s">
-        <v>218</v>
-      </c>
       <c r="E93" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F93" s="5" t="s">
         <v>33</v>
@@ -3295,16 +3292,16 @@
         <v>43852</v>
       </c>
       <c r="B94" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="C94" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D94" s="5" t="s">
-        <v>220</v>
-      </c>
       <c r="E94" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F94" s="5" t="s">
         <v>33</v>
@@ -3315,13 +3312,13 @@
         <v>43584</v>
       </c>
       <c r="B95" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D95" s="5" t="s">
-        <v>222</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>23</v>
@@ -3335,13 +3332,13 @@
         <v>43584</v>
       </c>
       <c r="B96" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D96" s="5" t="s">
-        <v>224</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>23</v>
@@ -3355,13 +3352,13 @@
         <v>43540</v>
       </c>
       <c r="B97" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>226</v>
       </c>
       <c r="E97" s="5" t="s">
         <v>23</v>
@@ -3372,7 +3369,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3380,16 +3377,16 @@
         <v>43203</v>
       </c>
       <c r="B99" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D99" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="C99" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D99" s="5" t="s">
-        <v>228</v>
-      </c>
       <c r="E99" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>77</v>
@@ -3400,19 +3397,19 @@
         <v>43203</v>
       </c>
       <c r="B100" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D100" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C100" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D100" s="5" t="s">
+      <c r="E100" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F100" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3420,13 +3417,13 @@
         <v>42842</v>
       </c>
       <c r="B101" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D101" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="C101" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D101" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>32</v>
@@ -3440,13 +3437,13 @@
         <v>42457</v>
       </c>
       <c r="B102" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D102" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>23</v>
@@ -3460,13 +3457,13 @@
         <v>39028</v>
       </c>
       <c r="B103" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" s="5" t="s">
         <v>236</v>
-      </c>
-      <c r="C103" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D103" s="5" t="s">
-        <v>237</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>32</v>
@@ -3637,10 +3634,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -3649,10 +3646,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: resolved OmegaT ticket #1519
</commit_message>
<xml_diff>
--- a/tickets/OmegaT_issues_nopw.xlsx
+++ b/tickets/OmegaT_issues_nopw.xlsx
@@ -1387,11 +1387,11 @@
   <dimension ref="A1:AMJ105"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+      <selection pane="bottomRight" activeCell="G55" activeCellId="0" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2984,7 +2984,7 @@
         <v>32</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added OmegaT RFE 1732
</commit_message>
<xml_diff>
--- a/tickets/OmegaT_issues_nopw.xlsx
+++ b/tickets/OmegaT_issues_nopw.xlsx
@@ -13,7 +13,7 @@
     <sheet name="ETS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$123</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'2022'!$A$1:$F$124</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="true" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="280">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -117,15 +117,24 @@
     <t xml:space="preserve">WIP</t>
   </si>
   <si>
+    <t xml:space="preserve">#1732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Commit target files" also commits exported master TM to repo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open!</t>
+  </si>
+  <si>
     <t xml:space="preserve">#1731</t>
   </si>
   <si>
     <t xml:space="preserve">Change label "Project translation" to "Committed target files"</t>
   </si>
   <si>
-    <t xml:space="preserve">RFE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Open</t>
   </si>
   <si>
@@ -133,9 +142,6 @@
   </si>
   <si>
     <t xml:space="preserve">Trim authentication details in team projects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open!</t>
   </si>
   <si>
     <t xml:space="preserve">#1724</t>
@@ -1441,14 +1447,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ125"/>
+  <dimension ref="A1:AMJ126"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1507,7 +1513,7 @@
     </row>
     <row r="4" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="n">
-        <v>45271</v>
+        <v>45274</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>30</v>
@@ -1531,7 +1537,7 @@
     </row>
     <row r="5" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="n">
-        <v>45238</v>
+        <v>45271</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>34</v>
@@ -1555,7 +1561,7 @@
     </row>
     <row r="6" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="n">
-        <v>45230</v>
+        <v>45238</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>37</v>
@@ -1570,7 +1576,7 @@
         <v>32</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
@@ -1579,7 +1585,7 @@
     </row>
     <row r="7" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
-        <v>45223</v>
+        <v>45230</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>39</v>
@@ -1603,7 +1609,7 @@
     </row>
     <row r="8" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
-        <v>45236</v>
+        <v>45223</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>41</v>
@@ -1615,10 +1621,10 @@
         <v>42</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="AMG8" s="0"/>
       <c r="AMH8" s="0"/>
@@ -1627,22 +1633,22 @@
     </row>
     <row r="9" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
-        <v>45233</v>
+        <v>45236</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="AMG9" s="0"/>
       <c r="AMH9" s="0"/>
@@ -1651,7 +1657,7 @@
     </row>
     <row r="10" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="n">
-        <v>45213</v>
+        <v>45233</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>46</v>
@@ -1663,7 +1669,7 @@
         <v>47</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>33</v>
@@ -1675,22 +1681,22 @@
     </row>
     <row r="11" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="n">
-        <v>45199</v>
+        <v>45213</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
@@ -1699,22 +1705,22 @@
     </row>
     <row r="12" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
-        <v>45170</v>
+        <v>45199</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>51</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -1723,7 +1729,7 @@
     </row>
     <row r="13" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="n">
-        <v>45169</v>
+        <v>45170</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>52</v>
@@ -1738,7 +1744,7 @@
         <v>32</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
@@ -1756,13 +1762,13 @@
         <v>7</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
@@ -1771,16 +1777,16 @@
     </row>
     <row r="15" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="n">
-        <v>45145</v>
+        <v>45169</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>9</v>
@@ -1810,7 +1816,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
@@ -1834,7 +1840,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
@@ -1843,16 +1849,22 @@
     </row>
     <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="n">
-        <v>45112</v>
+        <v>45145</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
@@ -1861,22 +1873,16 @@
     </row>
     <row r="19" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="n">
-        <v>45124</v>
-      </c>
-      <c r="B19" s="11" t="s">
+        <v>45112</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
@@ -1885,22 +1891,22 @@
     </row>
     <row r="20" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="n">
-        <v>45119</v>
+        <v>45124</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>65</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="E20" s="9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
@@ -1912,10 +1918,10 @@
         <v>45119</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>69</v>
@@ -1924,7 +1930,7 @@
         <v>32</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -1933,22 +1939,22 @@
     </row>
     <row r="22" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="n">
-        <v>45118</v>
+        <v>45119</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>71</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -1972,7 +1978,7 @@
         <v>9</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
@@ -1981,7 +1987,7 @@
     </row>
     <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="n">
-        <v>45110</v>
+        <v>45118</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>74</v>
@@ -1993,7 +1999,7 @@
         <v>75</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>33</v>
@@ -2005,7 +2011,7 @@
     </row>
     <row r="25" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="n">
-        <v>45104</v>
+        <v>45110</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>76</v>
@@ -2013,14 +2019,14 @@
       <c r="C25" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>41</v>
+      <c r="D25" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="AMG25" s="0"/>
       <c r="AMH25" s="0"/>
@@ -2029,22 +2035,22 @@
     </row>
     <row r="26" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="n">
-        <v>45094</v>
+        <v>45104</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>78</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>80</v>
+        <v>7</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AMG26" s="0"/>
       <c r="AMH26" s="0"/>
@@ -2053,13 +2059,13 @@
     </row>
     <row r="27" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="n">
-        <v>45069</v>
+        <v>45094</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>81</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>82</v>
@@ -2067,8 +2073,8 @@
       <c r="E27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>83</v>
+      <c r="F27" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="AMG27" s="0"/>
       <c r="AMH27" s="0"/>
@@ -2080,19 +2086,19 @@
         <v>45069</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>85</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="9" t="s">
-        <v>62</v>
+      <c r="F28" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="AMG28" s="0"/>
       <c r="AMH28" s="0"/>
@@ -2101,7 +2107,7 @@
     </row>
     <row r="29" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="n">
-        <v>45064</v>
+        <v>45069</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>86</v>
@@ -2116,7 +2122,7 @@
         <v>9</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="AMG29" s="0"/>
       <c r="AMH29" s="0"/>
@@ -2125,7 +2131,7 @@
     </row>
     <row r="30" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="n">
-        <v>45049</v>
+        <v>45064</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>88</v>
@@ -2139,8 +2145,8 @@
       <c r="E30" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="12" t="s">
-        <v>43</v>
+      <c r="F30" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="AMG30" s="0"/>
       <c r="AMH30" s="0"/>
@@ -2154,17 +2160,17 @@
       <c r="B31" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>79</v>
+      <c r="C31" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>91</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>62</v>
+        <v>9</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="AMG31" s="0"/>
       <c r="AMH31" s="0"/>
@@ -2173,22 +2179,22 @@
     </row>
     <row r="32" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="n">
-        <v>45044</v>
+        <v>45049</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>7</v>
+      <c r="C32" s="13" t="s">
+        <v>81</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AMG32" s="0"/>
       <c r="AMH32" s="0"/>
@@ -2197,7 +2203,7 @@
     </row>
     <row r="33" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="n">
-        <v>45040</v>
+        <v>45044</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>94</v>
@@ -2212,7 +2218,7 @@
         <v>9</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="AMG33" s="0"/>
       <c r="AMH33" s="0"/>
@@ -2221,7 +2227,7 @@
     </row>
     <row r="34" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="n">
-        <v>45028</v>
+        <v>45040</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>96</v>
@@ -2233,10 +2239,10 @@
         <v>97</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="AMG34" s="0"/>
       <c r="AMH34" s="0"/>
@@ -2245,16 +2251,22 @@
     </row>
     <row r="35" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="n">
-        <v>44996</v>
+        <v>45028</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>99</v>
       </c>
+      <c r="E35" s="9" t="s">
+        <v>32</v>
+      </c>
       <c r="F35" s="9" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="AMG35" s="0"/>
       <c r="AMH35" s="0"/>
@@ -2263,22 +2275,16 @@
     </row>
     <row r="36" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="n">
-        <v>45007</v>
-      </c>
-      <c r="B36" s="11" t="s">
+        <v>44996</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="F36" s="9" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="AMG36" s="0"/>
       <c r="AMH36" s="0"/>
@@ -2287,7 +2293,7 @@
     </row>
     <row r="37" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="n">
-        <v>44993</v>
+        <v>45007</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>102</v>
@@ -2302,7 +2308,7 @@
         <v>9</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
       <c r="AMG37" s="0"/>
       <c r="AMH37" s="0"/>
@@ -2326,7 +2332,7 @@
         <v>9</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AMG38" s="0"/>
       <c r="AMH38" s="0"/>
@@ -2335,22 +2341,22 @@
     </row>
     <row r="39" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="n">
-        <v>44991</v>
+        <v>44993</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>107</v>
+        <v>79</v>
       </c>
       <c r="AMG39" s="0"/>
       <c r="AMH39" s="0"/>
@@ -2359,22 +2365,22 @@
     </row>
     <row r="40" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="n">
-        <v>44981</v>
+        <v>44991</v>
       </c>
       <c r="B40" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="9" t="s">
+      <c r="E40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="AMG40" s="0"/>
       <c r="AMH40" s="0"/>
@@ -2383,7 +2389,7 @@
     </row>
     <row r="41" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="n">
-        <v>44972</v>
+        <v>44981</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>110</v>
@@ -2395,34 +2401,34 @@
         <v>111</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AMG41" s="0"/>
       <c r="AMH41" s="0"/>
       <c r="AMI41" s="0"/>
       <c r="AMJ41" s="0"/>
     </row>
-    <row r="42" s="16" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="n">
-        <v>44970</v>
-      </c>
-      <c r="B42" s="15" t="s">
+    <row r="42" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10" t="n">
+        <v>44972</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="13" t="s">
+      <c r="C42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="E42" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>33</v>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="AMG42" s="0"/>
       <c r="AMH42" s="0"/>
@@ -2431,13 +2437,13 @@
     </row>
     <row r="43" s="16" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="14" t="n">
-        <v>44967</v>
+        <v>44970</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>114</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="D43" s="13" t="s">
         <v>115</v>
@@ -2455,7 +2461,7 @@
     </row>
     <row r="44" s="16" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="14" t="n">
-        <v>44964</v>
+        <v>44967</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>116</v>
@@ -2470,7 +2476,7 @@
         <v>32</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="AMG44" s="0"/>
       <c r="AMH44" s="0"/>
@@ -2479,7 +2485,7 @@
     </row>
     <row r="45" s="16" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="14" t="n">
-        <v>44952</v>
+        <v>44964</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>118</v>
@@ -2494,7 +2500,7 @@
         <v>32</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AMG45" s="0"/>
       <c r="AMH45" s="0"/>
@@ -2518,7 +2524,7 @@
         <v>32</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="AMG46" s="0"/>
       <c r="AMH46" s="0"/>
@@ -2527,22 +2533,22 @@
     </row>
     <row r="47" s="16" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="14" t="n">
-        <v>44949</v>
+        <v>44952</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>122</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D47" s="13" t="s">
         <v>123</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="AMG47" s="0"/>
       <c r="AMH47" s="0"/>
@@ -2551,22 +2557,22 @@
     </row>
     <row r="48" s="16" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="14" t="n">
-        <v>44948</v>
+        <v>44949</v>
       </c>
       <c r="B48" s="15" t="s">
         <v>124</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>98</v>
+        <v>13</v>
       </c>
       <c r="D48" s="13" t="s">
         <v>125</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="AMG48" s="0"/>
       <c r="AMH48" s="0"/>
@@ -2575,130 +2581,130 @@
     </row>
     <row r="49" s="16" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="14" t="n">
-        <v>44946</v>
+        <v>44948</v>
       </c>
       <c r="B49" s="15" t="s">
         <v>126</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="D49" s="13" t="s">
         <v>127</v>
       </c>
       <c r="E49" s="13" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AMG49" s="0"/>
       <c r="AMH49" s="0"/>
       <c r="AMI49" s="0"/>
       <c r="AMJ49" s="0"/>
     </row>
-    <row r="50" s="13" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="16" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="14" t="n">
-        <v>44929</v>
-      </c>
-      <c r="B50" s="17" t="s">
+        <v>44946</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="13" t="s">
+      <c r="E50" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E50" s="13" t="s">
-        <v>128</v>
-      </c>
       <c r="F50" s="13" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="AMG50" s="0"/>
       <c r="AMH50" s="0"/>
       <c r="AMI50" s="0"/>
       <c r="AMJ50" s="0"/>
     </row>
-    <row r="51" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
+    <row r="51" s="13" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="14" t="n">
+        <v>44929</v>
+      </c>
+      <c r="B51" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="F51" s="8" t="s">
-        <v>29</v>
+      <c r="C51" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="AMG51" s="0"/>
       <c r="AMH51" s="0"/>
       <c r="AMI51" s="0"/>
       <c r="AMJ51" s="0"/>
     </row>
-    <row r="52" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="5" t="s">
+    <row r="52" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>33</v>
+      <c r="F52" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="AMG52" s="0"/>
       <c r="AMH52" s="0"/>
       <c r="AMI52" s="0"/>
       <c r="AMJ52" s="0"/>
     </row>
-    <row r="53" s="13" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="14" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B53" s="15" t="s">
+        <v>44879</v>
+      </c>
+      <c r="B53" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="C53" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="13" t="s">
+      <c r="C53" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E53" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F53" s="13" t="s">
-        <v>33</v>
+      <c r="E53" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="AMG53" s="0"/>
       <c r="AMH53" s="0"/>
       <c r="AMI53" s="0"/>
       <c r="AMJ53" s="0"/>
     </row>
-    <row r="54" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="13" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="14" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B54" s="18" t="s">
+        <v>44858</v>
+      </c>
+      <c r="B54" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="C54" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="E54" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>77</v>
+      <c r="E54" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="AMG54" s="0"/>
       <c r="AMH54" s="0"/>
@@ -2707,7 +2713,7 @@
     </row>
     <row r="55" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="14" t="n">
-        <v>44844</v>
+        <v>44855</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>138</v>
@@ -2719,113 +2725,117 @@
         <v>139</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="AMG55" s="0"/>
       <c r="AMH55" s="0"/>
       <c r="AMI55" s="0"/>
       <c r="AMJ55" s="0"/>
     </row>
-    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="8" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="14" t="n">
-        <v>44757</v>
-      </c>
-      <c r="B56" s="19" t="s">
+        <v>44844</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="E56" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F56" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="AMG56" s="0"/>
+      <c r="AMH56" s="0"/>
+      <c r="AMI56" s="0"/>
+      <c r="AMJ56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="14" t="n">
-        <v>373466</v>
-      </c>
-      <c r="B57" s="18" t="s">
+        <v>44757</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>7</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>145</v>
       </c>
       <c r="E57" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="14" t="n">
+        <v>373466</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F57" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="14" t="n">
+      <c r="F58" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="14" t="n">
         <v>44743</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="14" t="n">
-        <v>44740</v>
-      </c>
-      <c r="B59" s="20" t="s">
-        <v>147</v>
-      </c>
       <c r="C59" s="5" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E59" s="5" t="s">
-        <v>128</v>
-      </c>
       <c r="F59" s="5" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="14" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B60" s="21" t="s">
+        <v>44740</v>
+      </c>
+      <c r="B60" s="20" t="s">
         <v>149</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>150</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="14" t="n">
-        <v>44693</v>
+        <v>44739</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>151</v>
@@ -2837,77 +2847,77 @@
         <v>152</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="14" t="n">
-        <v>44695</v>
-      </c>
-      <c r="B62" s="22" t="s">
+        <v>44693</v>
+      </c>
+      <c r="B62" s="21" t="s">
         <v>153</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>154</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="14" t="n">
-        <v>44659</v>
+        <v>44695</v>
       </c>
       <c r="B63" s="22" t="s">
         <v>155</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>156</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="n">
-        <v>44712</v>
-      </c>
-      <c r="B64" s="21" t="s">
+        <v>44659</v>
+      </c>
+      <c r="B64" s="22" t="s">
         <v>157</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>158</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="14" t="n">
-        <v>44705</v>
-      </c>
-      <c r="B65" s="18" t="s">
+        <v>44712</v>
+      </c>
+      <c r="B65" s="21" t="s">
         <v>159</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2917,10 +2927,10 @@
         <v>160</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2937,15 +2947,15 @@
         <v>162</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="14" t="n">
-        <v>44693</v>
+        <v>44705</v>
       </c>
       <c r="B67" s="18" t="s">
         <v>163</v>
@@ -2957,15 +2967,15 @@
         <v>164</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="14" t="n">
-        <v>44622</v>
+        <v>44693</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>165</v>
@@ -2977,47 +2987,47 @@
         <v>166</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="14" t="n">
-        <v>44614</v>
+        <v>44622</v>
       </c>
       <c r="B69" s="18" t="s">
         <v>167</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>168</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="n">
-        <v>44613</v>
+        <v>44614</v>
       </c>
       <c r="B70" s="18" t="s">
         <v>169</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>170</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>33</v>
@@ -3025,9 +3035,9 @@
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="14" t="n">
-        <v>44608</v>
-      </c>
-      <c r="B71" s="21" t="s">
+        <v>44613</v>
+      </c>
+      <c r="B71" s="18" t="s">
         <v>171</v>
       </c>
       <c r="C71" s="5" t="s">
@@ -3037,60 +3047,60 @@
         <v>172</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="14" t="n">
-        <v>44580</v>
-      </c>
-      <c r="B72" s="18" t="s">
+        <v>44608</v>
+      </c>
+      <c r="B72" s="21" t="s">
         <v>173</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E72" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F72" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="14" t="n">
+        <v>44580</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F72" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="14" t="n">
-        <v>44463</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D74" s="5" t="s">
+      <c r="F73" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="14" t="n">
-        <v>44460</v>
+        <v>44463</v>
       </c>
       <c r="B75" s="18" t="s">
         <v>178</v>
@@ -3102,10 +3112,10 @@
         <v>179</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>180</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3113,24 +3123,24 @@
         <v>44460</v>
       </c>
       <c r="B76" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D76" s="5" t="s">
+      <c r="E76" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F76" s="5" t="s">
         <v>182</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="14" t="n">
-        <v>44372</v>
+        <v>44460</v>
       </c>
       <c r="B77" s="18" t="s">
         <v>183</v>
@@ -3145,64 +3155,64 @@
         <v>23</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="14" t="n">
-        <v>44326</v>
+        <v>44372</v>
       </c>
       <c r="B78" s="18" t="s">
         <v>185</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>142</v>
+        <v>7</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>186</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>140</v>
+        <v>36</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="14" t="n">
-        <v>44325</v>
-      </c>
-      <c r="B79" s="22" t="s">
+        <v>44326</v>
+      </c>
+      <c r="B79" s="18" t="s">
         <v>187</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>188</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="14" t="n">
         <v>44325</v>
       </c>
-      <c r="B80" s="18" t="s">
+      <c r="B80" s="22" t="s">
         <v>189</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>190</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="F80" s="5" t="s">
         <v>33</v>
@@ -3210,7 +3220,7 @@
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="14" t="n">
-        <v>44321</v>
+        <v>44325</v>
       </c>
       <c r="B81" s="18" t="s">
         <v>191</v>
@@ -3222,15 +3232,15 @@
         <v>192</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="14" t="n">
-        <v>44316</v>
+        <v>44321</v>
       </c>
       <c r="B82" s="18" t="s">
         <v>193</v>
@@ -3242,37 +3252,37 @@
         <v>194</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>195</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="14" t="n">
-        <v>44279</v>
-      </c>
-      <c r="B83" s="5" t="s">
+        <v>44316</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C83" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D83" s="5" t="s">
+      <c r="E83" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F83" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="14" t="n">
-        <v>44257</v>
-      </c>
-      <c r="B84" s="18" t="s">
+        <v>44279</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>198</v>
       </c>
       <c r="C84" s="5" t="s">
@@ -3282,7 +3292,7 @@
         <v>199</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>33</v>
@@ -3290,7 +3300,7 @@
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="14" t="n">
-        <v>44243</v>
+        <v>44257</v>
       </c>
       <c r="B85" s="18" t="s">
         <v>200</v>
@@ -3302,57 +3312,57 @@
         <v>201</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="23" t="n">
+      <c r="A86" s="14" t="n">
+        <v>44243</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="23" t="n">
         <v>44231</v>
       </c>
-      <c r="B86" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="C86" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D86" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="E86" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="F86" s="25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="14" t="n">
-        <v>44218</v>
-      </c>
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" s="5" t="s">
+      <c r="C87" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="E87" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F87" s="25" t="s">
         <v>205</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="14" t="n">
-        <v>44216</v>
-      </c>
-      <c r="B88" s="21" t="s">
+        <v>44218</v>
+      </c>
+      <c r="B88" s="18" t="s">
         <v>206</v>
       </c>
       <c r="C88" s="5" t="s">
@@ -3362,7 +3372,7 @@
         <v>207</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="F88" s="5" t="s">
         <v>36</v>
@@ -3370,9 +3380,9 @@
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="14" t="n">
-        <v>44175</v>
-      </c>
-      <c r="B89" s="18" t="s">
+        <v>44216</v>
+      </c>
+      <c r="B89" s="21" t="s">
         <v>208</v>
       </c>
       <c r="C89" s="5" t="s">
@@ -3382,7 +3392,7 @@
         <v>209</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="F89" s="5" t="s">
         <v>33</v>
@@ -3402,40 +3412,40 @@
         <v>211</v>
       </c>
       <c r="E90" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="14" t="n">
+        <v>44175</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E91" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F90" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="14" t="n">
-        <v>44162</v>
-      </c>
-      <c r="B92" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="C92" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D92" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F92" s="5" t="s">
-        <v>33</v>
+      <c r="F91" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="5" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="14" t="n">
-        <v>44148</v>
+        <v>44162</v>
       </c>
       <c r="B93" s="18" t="s">
         <v>214</v>
@@ -3444,124 +3454,124 @@
         <v>7</v>
       </c>
       <c r="D93" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="14" t="n">
+        <v>44148</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="23" t="n">
+      <c r="E94" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="23" t="n">
         <v>44146</v>
       </c>
-      <c r="B94" s="24" t="s">
-        <v>215</v>
-      </c>
-      <c r="C94" s="25" t="s">
+      <c r="B95" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C95" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D94" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="E94" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="F94" s="25" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="14" t="n">
-        <v>44132</v>
-      </c>
-      <c r="B95" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="E95" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>33</v>
+      <c r="E95" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F95" s="25" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="14" t="n">
-        <v>44103</v>
+        <v>44132</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>220</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="23" t="n">
+      <c r="A97" s="14" t="n">
+        <v>44103</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="23" t="n">
         <v>44095</v>
       </c>
-      <c r="B97" s="24" t="s">
-        <v>221</v>
-      </c>
-      <c r="C97" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D97" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="E97" s="25" t="s">
+      <c r="B98" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="C98" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="E98" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F97" s="25" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="14" t="n">
-        <v>44095</v>
-      </c>
-      <c r="B98" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D98" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>62</v>
+      <c r="F98" s="25" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="14" t="n">
-        <v>44057</v>
+        <v>44095</v>
       </c>
       <c r="B99" s="18" t="s">
         <v>225</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>226</v>
@@ -3570,32 +3580,32 @@
         <v>32</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>180</v>
+        <v>64</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="14" t="n">
-        <v>44028</v>
+        <v>44057</v>
       </c>
       <c r="B100" s="18" t="s">
         <v>227</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>228</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>62</v>
+        <v>182</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="14" t="n">
-        <v>44064</v>
+        <v>44028</v>
       </c>
       <c r="B101" s="18" t="s">
         <v>229</v>
@@ -3607,15 +3617,15 @@
         <v>230</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="14" t="n">
-        <v>44028</v>
+        <v>44064</v>
       </c>
       <c r="B102" s="18" t="s">
         <v>231</v>
@@ -3627,15 +3637,15 @@
         <v>232</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="14" t="n">
-        <v>44016</v>
+        <v>44028</v>
       </c>
       <c r="B103" s="18" t="s">
         <v>233</v>
@@ -3647,15 +3657,15 @@
         <v>234</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="14" t="n">
-        <v>44010</v>
+        <v>44016</v>
       </c>
       <c r="B104" s="18" t="s">
         <v>235</v>
@@ -3667,35 +3677,35 @@
         <v>236</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="14" t="n">
-        <v>43995</v>
+        <v>44010</v>
       </c>
       <c r="B105" s="18" t="s">
         <v>237</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>238</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="14" t="n">
-        <v>43948</v>
+        <v>43995</v>
       </c>
       <c r="B106" s="18" t="s">
         <v>239</v>
@@ -3707,15 +3717,15 @@
         <v>240</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="14" t="n">
-        <v>43947</v>
+        <v>43948</v>
       </c>
       <c r="B107" s="18" t="s">
         <v>241</v>
@@ -3727,15 +3737,15 @@
         <v>242</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="14" t="n">
-        <v>43936</v>
+        <v>43947</v>
       </c>
       <c r="B108" s="18" t="s">
         <v>243</v>
@@ -3747,7 +3757,7 @@
         <v>244</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>32</v>
+        <v>130</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>33</v>
@@ -3755,27 +3765,27 @@
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="14" t="n">
-        <v>43929</v>
+        <v>43936</v>
       </c>
       <c r="B109" s="18" t="s">
         <v>245</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>246</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="14" t="n">
-        <v>43891</v>
+        <v>43929</v>
       </c>
       <c r="B110" s="18" t="s">
         <v>247</v>
@@ -3787,15 +3797,15 @@
         <v>248</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="14" t="n">
-        <v>43885</v>
+        <v>43891</v>
       </c>
       <c r="B111" s="18" t="s">
         <v>249</v>
@@ -3807,15 +3817,15 @@
         <v>250</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="14" t="n">
-        <v>43857</v>
+        <v>43885</v>
       </c>
       <c r="B112" s="18" t="s">
         <v>251</v>
@@ -3827,10 +3837,10 @@
         <v>252</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3847,15 +3857,15 @@
         <v>254</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="14" t="n">
-        <v>43852</v>
+        <v>43857</v>
       </c>
       <c r="B114" s="18" t="s">
         <v>255</v>
@@ -3867,15 +3877,15 @@
         <v>256</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="14" t="n">
-        <v>43584</v>
+        <v>43852</v>
       </c>
       <c r="B115" s="18" t="s">
         <v>257</v>
@@ -3887,10 +3897,10 @@
         <v>258</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>23</v>
+        <v>130</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3910,14 +3920,14 @@
         <v>23</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="14" t="n">
-        <v>43540</v>
-      </c>
-      <c r="B117" s="5" t="s">
+        <v>43584</v>
+      </c>
+      <c r="B117" s="18" t="s">
         <v>261</v>
       </c>
       <c r="C117" s="5" t="s">
@@ -3930,32 +3940,32 @@
         <v>23</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="5" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="14" t="n">
-        <v>43203</v>
-      </c>
-      <c r="B119" s="26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="14" t="n">
+        <v>43540</v>
+      </c>
+      <c r="B118" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C119" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D119" s="5" t="s">
+      <c r="C118" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="E119" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>36</v>
+      <c r="E118" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="5" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3966,53 +3976,53 @@
         <v>265</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>266</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>267</v>
+        <v>33</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="14" t="n">
-        <v>42842</v>
+        <v>43203</v>
       </c>
       <c r="B121" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D121" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="C121" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D121" s="5" t="s">
+      <c r="E121" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F121" s="5" t="s">
         <v>269</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="14" t="n">
-        <v>42457</v>
-      </c>
-      <c r="B122" s="5" t="s">
+        <v>42842</v>
+      </c>
+      <c r="B122" s="26" t="s">
         <v>270</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>271</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F122" s="5" t="s">
         <v>33</v>
@@ -4020,7 +4030,7 @@
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="14" t="n">
-        <v>39028</v>
+        <v>42457</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>272</v>
@@ -4032,135 +4042,156 @@
         <v>273</v>
       </c>
       <c r="E123" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="14" t="n">
+        <v>39028</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="E124" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F123" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="125" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="AMG125" s="0"/>
-      <c r="AMH125" s="0"/>
-      <c r="AMI125" s="0"/>
-      <c r="AMJ125" s="0"/>
+      <c r="F124" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AMG126" s="0"/>
+      <c r="AMH126" s="0"/>
+      <c r="AMI126" s="0"/>
+      <c r="AMJ126" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F123"/>
+  <autoFilter ref="A1:F124"/>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="#1731"/>
-    <hyperlink ref="B5" r:id="rId2" display="#1725"/>
-    <hyperlink ref="B6" r:id="rId3" display="#1724"/>
-    <hyperlink ref="B7" r:id="rId4" display="#1722"/>
-    <hyperlink ref="B8" r:id="rId5" display="#1226"/>
-    <hyperlink ref="B9" r:id="rId6" display="#1225"/>
-    <hyperlink ref="B10" r:id="rId7" display="#1720"/>
-    <hyperlink ref="B11" r:id="rId8" display="#1323"/>
-    <hyperlink ref="B12" r:id="rId9" display="#30"/>
-    <hyperlink ref="B13" r:id="rId10" display="#1712"/>
-    <hyperlink ref="B14" r:id="rId11" display="#1215"/>
-    <hyperlink ref="B15" r:id="rId12" display="#1214"/>
-    <hyperlink ref="B16" r:id="rId13" display="#1213"/>
-    <hyperlink ref="B17" r:id="rId14" display="#1212"/>
-    <hyperlink ref="B19" r:id="rId15" display="#1202"/>
-    <hyperlink ref="B20" r:id="rId16" display="#27"/>
-    <hyperlink ref="B21" r:id="rId17" display="#26"/>
-    <hyperlink ref="B22" r:id="rId18" display="#1201"/>
-    <hyperlink ref="B23" r:id="rId19" display="#1200"/>
-    <hyperlink ref="B24" r:id="rId20" display="#1708"/>
-    <hyperlink ref="B25" r:id="rId21" display="#1185"/>
-    <hyperlink ref="D25" r:id="rId22" display="#1226"/>
-    <hyperlink ref="B26" r:id="rId23" display="#11"/>
-    <hyperlink ref="B27" r:id="rId24" display="#1309"/>
-    <hyperlink ref="B28" r:id="rId25" display="#1176"/>
-    <hyperlink ref="B29" r:id="rId26" display="#1171"/>
-    <hyperlink ref="B30" r:id="rId27" display="#1164"/>
-    <hyperlink ref="B31" r:id="rId28" display="#9"/>
-    <hyperlink ref="B32" r:id="rId29" display="#1163"/>
-    <hyperlink ref="B33" r:id="rId30" display="#1161"/>
-    <hyperlink ref="B34" r:id="rId31" display="#1690"/>
-    <hyperlink ref="B36" r:id="rId32" display="#1155"/>
-    <hyperlink ref="B37" r:id="rId33" display="#1150"/>
-    <hyperlink ref="B38" r:id="rId34" display="#1151"/>
-    <hyperlink ref="B39" r:id="rId35" display="#1200"/>
-    <hyperlink ref="B40" r:id="rId36" display="#1681"/>
-    <hyperlink ref="B41" r:id="rId37" display="#1142"/>
-    <hyperlink ref="B42" r:id="rId38" display="#8"/>
-    <hyperlink ref="B43" r:id="rId39" display="#1674"/>
-    <hyperlink ref="B44" r:id="rId40" display="#1672"/>
-    <hyperlink ref="B45" r:id="rId41" display="#1669"/>
-    <hyperlink ref="B46" r:id="rId42" display="#1670"/>
-    <hyperlink ref="B47" r:id="rId43" display="#1184"/>
-    <hyperlink ref="B48" r:id="rId44" display="#49"/>
-    <hyperlink ref="B49" r:id="rId45" display="#1140"/>
-    <hyperlink ref="B50" r:id="rId46" display="#1132"/>
-    <hyperlink ref="B52" r:id="rId47" display="#1125"/>
-    <hyperlink ref="B53" r:id="rId48" display="#1641"/>
-    <hyperlink ref="B54" r:id="rId49" display="#1124"/>
-    <hyperlink ref="B55" r:id="rId50" display="#1122"/>
-    <hyperlink ref="B56" r:id="rId51" display="#43"/>
-    <hyperlink ref="B57" r:id="rId52" display="#1622"/>
-    <hyperlink ref="B59" r:id="rId53" display="#38"/>
-    <hyperlink ref="B60" r:id="rId54" display="#1621"/>
-    <hyperlink ref="B61" r:id="rId55" display="#1616"/>
-    <hyperlink ref="B62" r:id="rId56" display="#37"/>
-    <hyperlink ref="B63" r:id="rId57" display="#36"/>
-    <hyperlink ref="B64" r:id="rId58" display="#1101"/>
-    <hyperlink ref="B65" r:id="rId59" display="#1099"/>
-    <hyperlink ref="B66" r:id="rId60" display="#1098"/>
-    <hyperlink ref="B67" r:id="rId61" display="#1617"/>
-    <hyperlink ref="B68" r:id="rId62" display="#1092"/>
-    <hyperlink ref="B69" r:id="rId63" display="#1128"/>
-    <hyperlink ref="B70" r:id="rId64" display="#1090"/>
-    <hyperlink ref="B71" r:id="rId65" display="#1608"/>
-    <hyperlink ref="B72" r:id="rId66" display="#35"/>
-    <hyperlink ref="B74" r:id="rId67" display="#1070"/>
-    <hyperlink ref="B75" r:id="rId68" display="#1592"/>
-    <hyperlink ref="B76" r:id="rId69" display="#1591"/>
-    <hyperlink ref="B77" r:id="rId70" display="#1578"/>
-    <hyperlink ref="B78" r:id="rId71" display="#41"/>
-    <hyperlink ref="B79" r:id="rId72" display="#42"/>
-    <hyperlink ref="B80" r:id="rId73" display="#1566"/>
-    <hyperlink ref="B81" r:id="rId74" display="#1565"/>
-    <hyperlink ref="B82" r:id="rId75" display="#1046"/>
-    <hyperlink ref="B83" r:id="rId76" display="#1559"/>
-    <hyperlink ref="B84" r:id="rId77" display="#1038"/>
-    <hyperlink ref="B85" r:id="rId78" display="#1037"/>
-    <hyperlink ref="B86" r:id="rId79" display="#1020"/>
-    <hyperlink ref="B87" r:id="rId80" display="#1032"/>
-    <hyperlink ref="B88" r:id="rId81" display="#1546"/>
-    <hyperlink ref="B89" r:id="rId82" display="#1027"/>
-    <hyperlink ref="B90" r:id="rId83" display="#1529"/>
-    <hyperlink ref="B92" r:id="rId84" display="#1527"/>
-    <hyperlink ref="B93" r:id="rId85" display="#558"/>
-    <hyperlink ref="B94" r:id="rId86" display="#1005"/>
-    <hyperlink ref="B95" r:id="rId87" display="#1020"/>
-    <hyperlink ref="B96" r:id="rId88" display="#993"/>
-    <hyperlink ref="B97" r:id="rId89" display="#1520"/>
-    <hyperlink ref="B98" r:id="rId90" display="#1519"/>
-    <hyperlink ref="B99" r:id="rId91" display="#969"/>
-    <hyperlink ref="B100" r:id="rId92" display="#1003"/>
-    <hyperlink ref="B101" r:id="rId93" display="#1015"/>
-    <hyperlink ref="B102" r:id="rId94" display="#1002"/>
-    <hyperlink ref="B103" r:id="rId95" display="#1471"/>
-    <hyperlink ref="B104" r:id="rId96" display="#1497"/>
-    <hyperlink ref="B105" r:id="rId97" display="#947"/>
-    <hyperlink ref="B106" r:id="rId98" display="#933"/>
-    <hyperlink ref="B107" r:id="rId99" display="#932"/>
-    <hyperlink ref="B108" r:id="rId100" display="#931"/>
-    <hyperlink ref="B109" r:id="rId101" display="#987"/>
-    <hyperlink ref="B110" r:id="rId102" display="#988"/>
-    <hyperlink ref="B111" r:id="rId103" display="#982"/>
-    <hyperlink ref="B112" r:id="rId104" display="#979"/>
-    <hyperlink ref="B113" r:id="rId105" display="#977"/>
-    <hyperlink ref="B114" r:id="rId106" display="#975"/>
-    <hyperlink ref="B115" r:id="rId107" display="#1445"/>
-    <hyperlink ref="B116" r:id="rId108" display="#1444"/>
-    <hyperlink ref="B117" r:id="rId109" display="#1427"/>
-    <hyperlink ref="B119" r:id="rId110" display="#23"/>
-    <hyperlink ref="B120" r:id="rId111" display="#22"/>
-    <hyperlink ref="B121" r:id="rId112" display="#18"/>
-    <hyperlink ref="B122" r:id="rId113" display="#1207"/>
-    <hyperlink ref="B123" r:id="rId114" display="#245"/>
+    <hyperlink ref="B4" r:id="rId1" display="#1732"/>
+    <hyperlink ref="B5" r:id="rId2" display="#1731"/>
+    <hyperlink ref="B6" r:id="rId3" display="#1725"/>
+    <hyperlink ref="B7" r:id="rId4" display="#1724"/>
+    <hyperlink ref="B8" r:id="rId5" display="#1722"/>
+    <hyperlink ref="B9" r:id="rId6" display="#1226"/>
+    <hyperlink ref="B10" r:id="rId7" display="#1225"/>
+    <hyperlink ref="B11" r:id="rId8" display="#1720"/>
+    <hyperlink ref="B12" r:id="rId9" display="#1323"/>
+    <hyperlink ref="B13" r:id="rId10" display="#30"/>
+    <hyperlink ref="B14" r:id="rId11" display="#1712"/>
+    <hyperlink ref="B15" r:id="rId12" display="#1215"/>
+    <hyperlink ref="B16" r:id="rId13" display="#1214"/>
+    <hyperlink ref="B17" r:id="rId14" display="#1213"/>
+    <hyperlink ref="B18" r:id="rId15" display="#1212"/>
+    <hyperlink ref="B20" r:id="rId16" display="#1202"/>
+    <hyperlink ref="B21" r:id="rId17" display="#27"/>
+    <hyperlink ref="B22" r:id="rId18" display="#26"/>
+    <hyperlink ref="B23" r:id="rId19" display="#1201"/>
+    <hyperlink ref="B24" r:id="rId20" display="#1200"/>
+    <hyperlink ref="B25" r:id="rId21" display="#1708"/>
+    <hyperlink ref="B26" r:id="rId22" display="#1185"/>
+    <hyperlink ref="D26" r:id="rId23" display="#1226"/>
+    <hyperlink ref="B27" r:id="rId24" display="#11"/>
+    <hyperlink ref="B28" r:id="rId25" display="#1309"/>
+    <hyperlink ref="B29" r:id="rId26" display="#1176"/>
+    <hyperlink ref="B30" r:id="rId27" display="#1171"/>
+    <hyperlink ref="B31" r:id="rId28" display="#1164"/>
+    <hyperlink ref="B32" r:id="rId29" display="#9"/>
+    <hyperlink ref="B33" r:id="rId30" display="#1163"/>
+    <hyperlink ref="B34" r:id="rId31" display="#1161"/>
+    <hyperlink ref="B35" r:id="rId32" display="#1690"/>
+    <hyperlink ref="B37" r:id="rId33" display="#1155"/>
+    <hyperlink ref="B38" r:id="rId34" display="#1150"/>
+    <hyperlink ref="B39" r:id="rId35" display="#1151"/>
+    <hyperlink ref="B40" r:id="rId36" display="#1200"/>
+    <hyperlink ref="B41" r:id="rId37" display="#1681"/>
+    <hyperlink ref="B42" r:id="rId38" display="#1142"/>
+    <hyperlink ref="B43" r:id="rId39" display="#8"/>
+    <hyperlink ref="B44" r:id="rId40" display="#1674"/>
+    <hyperlink ref="B45" r:id="rId41" display="#1672"/>
+    <hyperlink ref="B46" r:id="rId42" display="#1669"/>
+    <hyperlink ref="B47" r:id="rId43" display="#1670"/>
+    <hyperlink ref="B48" r:id="rId44" display="#1184"/>
+    <hyperlink ref="B49" r:id="rId45" display="#49"/>
+    <hyperlink ref="B50" r:id="rId46" display="#1140"/>
+    <hyperlink ref="B51" r:id="rId47" display="#1132"/>
+    <hyperlink ref="B53" r:id="rId48" display="#1125"/>
+    <hyperlink ref="B54" r:id="rId49" display="#1641"/>
+    <hyperlink ref="B55" r:id="rId50" display="#1124"/>
+    <hyperlink ref="B56" r:id="rId51" display="#1122"/>
+    <hyperlink ref="B57" r:id="rId52" display="#43"/>
+    <hyperlink ref="B58" r:id="rId53" display="#1622"/>
+    <hyperlink ref="B60" r:id="rId54" display="#38"/>
+    <hyperlink ref="B61" r:id="rId55" display="#1621"/>
+    <hyperlink ref="B62" r:id="rId56" display="#1616"/>
+    <hyperlink ref="B63" r:id="rId57" display="#37"/>
+    <hyperlink ref="B64" r:id="rId58" display="#36"/>
+    <hyperlink ref="B65" r:id="rId59" display="#1101"/>
+    <hyperlink ref="B66" r:id="rId60" display="#1099"/>
+    <hyperlink ref="B67" r:id="rId61" display="#1098"/>
+    <hyperlink ref="B68" r:id="rId62" display="#1617"/>
+    <hyperlink ref="B69" r:id="rId63" display="#1092"/>
+    <hyperlink ref="B70" r:id="rId64" display="#1128"/>
+    <hyperlink ref="B71" r:id="rId65" display="#1090"/>
+    <hyperlink ref="B72" r:id="rId66" display="#1608"/>
+    <hyperlink ref="B73" r:id="rId67" display="#35"/>
+    <hyperlink ref="B75" r:id="rId68" display="#1070"/>
+    <hyperlink ref="B76" r:id="rId69" display="#1592"/>
+    <hyperlink ref="B77" r:id="rId70" display="#1591"/>
+    <hyperlink ref="B78" r:id="rId71" display="#1578"/>
+    <hyperlink ref="B79" r:id="rId72" display="#41"/>
+    <hyperlink ref="B80" r:id="rId73" display="#42"/>
+    <hyperlink ref="B81" r:id="rId74" display="#1566"/>
+    <hyperlink ref="B82" r:id="rId75" display="#1565"/>
+    <hyperlink ref="B83" r:id="rId76" display="#1046"/>
+    <hyperlink ref="B84" r:id="rId77" display="#1559"/>
+    <hyperlink ref="B85" r:id="rId78" display="#1038"/>
+    <hyperlink ref="B86" r:id="rId79" display="#1037"/>
+    <hyperlink ref="B87" r:id="rId80" display="#1020"/>
+    <hyperlink ref="B88" r:id="rId81" display="#1032"/>
+    <hyperlink ref="B89" r:id="rId82" display="#1546"/>
+    <hyperlink ref="B90" r:id="rId83" display="#1027"/>
+    <hyperlink ref="B91" r:id="rId84" display="#1529"/>
+    <hyperlink ref="B93" r:id="rId85" display="#1527"/>
+    <hyperlink ref="B94" r:id="rId86" display="#558"/>
+    <hyperlink ref="B95" r:id="rId87" display="#1005"/>
+    <hyperlink ref="B96" r:id="rId88" display="#1020"/>
+    <hyperlink ref="B97" r:id="rId89" display="#993"/>
+    <hyperlink ref="B98" r:id="rId90" display="#1520"/>
+    <hyperlink ref="B99" r:id="rId91" display="#1519"/>
+    <hyperlink ref="B100" r:id="rId92" display="#969"/>
+    <hyperlink ref="B101" r:id="rId93" display="#1003"/>
+    <hyperlink ref="B102" r:id="rId94" display="#1015"/>
+    <hyperlink ref="B103" r:id="rId95" display="#1002"/>
+    <hyperlink ref="B104" r:id="rId96" display="#1471"/>
+    <hyperlink ref="B105" r:id="rId97" display="#1497"/>
+    <hyperlink ref="B106" r:id="rId98" display="#947"/>
+    <hyperlink ref="B107" r:id="rId99" display="#933"/>
+    <hyperlink ref="B108" r:id="rId100" display="#932"/>
+    <hyperlink ref="B109" r:id="rId101" display="#931"/>
+    <hyperlink ref="B110" r:id="rId102" display="#987"/>
+    <hyperlink ref="B111" r:id="rId103" display="#988"/>
+    <hyperlink ref="B112" r:id="rId104" display="#982"/>
+    <hyperlink ref="B113" r:id="rId105" display="#979"/>
+    <hyperlink ref="B114" r:id="rId106" display="#977"/>
+    <hyperlink ref="B115" r:id="rId107" display="#975"/>
+    <hyperlink ref="B116" r:id="rId108" display="#1445"/>
+    <hyperlink ref="B117" r:id="rId109" display="#1444"/>
+    <hyperlink ref="B118" r:id="rId110" display="#1427"/>
+    <hyperlink ref="B120" r:id="rId111" display="#23"/>
+    <hyperlink ref="B121" r:id="rId112" display="#22"/>
+    <hyperlink ref="B122" r:id="rId113" display="#18"/>
+    <hyperlink ref="B123" r:id="rId114" display="#1207"/>
+    <hyperlink ref="B124" r:id="rId115" display="#245"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="1" footer="1"/>
@@ -4169,7 +4200,7 @@
     <oddHeader>&amp;C&amp;"Sans,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Sans,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId115"/>
+  <drawing r:id="rId116"/>
 </worksheet>
 </file>
 
@@ -4202,10 +4233,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -4214,10 +4245,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>